<commit_message>
Latest update to the Metrics
</commit_message>
<xml_diff>
--- a/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
+++ b/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\Output\April_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620BE717-967B-45D4-935D-F7B8C7CD8784}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A801DDC-DF8D-440E-BED7-E230DDEF27B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18270" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="18270" windowHeight="13695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMA Reason Codes" sheetId="1" r:id="rId1"/>
     <sheet name="Driver and Engine RMAs" sheetId="3" r:id="rId2"/>
     <sheet name="YTD" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="185">
   <si>
     <t># of RMAs</t>
   </si>
@@ -998,6 +997,12 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1018,12 +1023,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6695,7 +6694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7600A-0572-4151-919D-5CF8CE548ABA}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -6731,28 +6730,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49"/>
       <c r="S1" s="32"/>
       <c r="U1" s="23"/>
       <c r="V1" s="23"/>
@@ -6833,16 +6832,16 @@
       <c r="D3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="45">
         <v>13.25</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="45">
         <v>45</v>
       </c>
-      <c r="G3" s="52">
+      <c r="G3" s="45">
         <v>1350</v>
       </c>
-      <c r="H3" s="53"/>
+      <c r="H3" s="46"/>
       <c r="I3" s="5"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -6890,13 +6889,13 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="45">
         <v>12.3</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="45">
         <v>38</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="45">
         <v>950</v>
       </c>
       <c r="H4" s="5"/>
@@ -6947,13 +6946,13 @@
       <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="45">
         <v>15</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="45">
         <v>52</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="45">
         <v>832</v>
       </c>
       <c r="H5" s="5"/>
@@ -7004,13 +7003,13 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="45">
         <v>12.67</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="45">
         <v>45</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="45">
         <v>630</v>
       </c>
       <c r="H6" s="5"/>
@@ -7061,13 +7060,13 @@
       <c r="D7" s="3">
         <v>22</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="45">
         <v>11.99</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="45">
         <v>48</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="45">
         <v>624</v>
       </c>
       <c r="H7" s="5"/>
@@ -7118,13 +7117,13 @@
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="45">
         <v>45.39</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="45">
         <v>114</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="45">
         <v>1368</v>
       </c>
       <c r="H8" s="5"/>
@@ -7175,13 +7174,13 @@
       <c r="D9" s="3">
         <v>19</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="45">
         <v>18.9618</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="45">
         <v>50</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="45">
         <v>600</v>
       </c>
       <c r="H9" s="5"/>
@@ -7232,13 +7231,13 @@
       <c r="D10" s="3">
         <v>22</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="45">
         <v>11.986000000000001</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="45">
         <v>42</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="45">
         <v>420</v>
       </c>
       <c r="H10" s="5"/>
@@ -7289,13 +7288,13 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="45">
         <v>14.208600000000001</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="45">
         <v>44</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="45">
         <v>352</v>
       </c>
       <c r="H11" s="5"/>
@@ -7346,13 +7345,13 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="45">
         <v>12.67</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="45">
         <v>43</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="45">
         <v>301</v>
       </c>
       <c r="H12" s="5"/>
@@ -7403,13 +7402,13 @@
       <c r="D13" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="45">
         <v>40</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="45">
         <v>133</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G13" s="45">
         <v>665</v>
       </c>
       <c r="H13" s="5"/>
@@ -7460,13 +7459,13 @@
       <c r="D14" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="45">
         <v>35.19</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="45">
         <v>98</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="45">
         <v>490</v>
       </c>
       <c r="H14" s="5"/>
@@ -7517,13 +7516,13 @@
       <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="45">
         <v>15.72</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="45">
         <v>49</v>
       </c>
-      <c r="G15" s="52">
+      <c r="G15" s="45">
         <v>196</v>
       </c>
       <c r="H15" s="5"/>
@@ -7574,13 +7573,13 @@
       <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="45">
         <v>14.555400000000001</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="45">
         <v>55</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G16" s="45">
         <v>220</v>
       </c>
       <c r="H16" s="5"/>
@@ -7631,13 +7630,13 @@
       <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="45">
         <v>40</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F17" s="45">
         <v>112</v>
       </c>
-      <c r="G17" s="52">
+      <c r="G17" s="45">
         <v>336</v>
       </c>
       <c r="H17" s="5"/>
@@ -7688,13 +7687,13 @@
       <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="45">
         <v>45.39</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="45">
         <v>117</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="45">
         <v>351</v>
       </c>
       <c r="H18" s="5"/>
@@ -7745,13 +7744,13 @@
       <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="45">
         <v>15.72</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="45">
         <v>46</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="45">
         <v>138</v>
       </c>
       <c r="H19" s="5"/>
@@ -7802,13 +7801,13 @@
       <c r="D20" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="45">
         <v>24</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="45">
         <v>75</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="45">
         <v>225</v>
       </c>
       <c r="H20" s="5"/>
@@ -7859,13 +7858,13 @@
       <c r="D21" s="3">
         <v>22</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="45">
         <v>12.19</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="45">
         <v>39</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G21" s="45">
         <v>117</v>
       </c>
       <c r="H21" s="5"/>
@@ -7916,13 +7915,13 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="45">
         <v>17.649999999999999</v>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="45">
         <v>87</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="45">
         <v>174</v>
       </c>
       <c r="H22" s="5"/>
@@ -7973,13 +7972,13 @@
       <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="45">
         <v>45.39</v>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="45">
         <v>115</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="45">
         <v>230</v>
       </c>
       <c r="H23" s="5"/>
@@ -8030,13 +8029,13 @@
       <c r="D24" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="45">
         <v>23</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="45">
         <v>79</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="45">
         <v>158</v>
       </c>
       <c r="H24" s="5"/>
@@ -8087,13 +8086,13 @@
       <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="45">
         <v>15.72</v>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="45">
         <v>39</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="45">
         <v>78</v>
       </c>
       <c r="H25" s="5"/>
@@ -8144,13 +8143,13 @@
       <c r="D26" s="3">
         <v>2</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="45">
         <v>14.31</v>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="45">
         <v>52</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="45">
         <v>104</v>
       </c>
       <c r="H26" s="5"/>
@@ -8201,13 +8200,13 @@
       <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="45">
         <v>14.31</v>
       </c>
-      <c r="F27" s="52">
+      <c r="F27" s="45">
         <v>54</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="45">
         <v>108</v>
       </c>
       <c r="H27" s="5"/>
@@ -8258,13 +8257,13 @@
       <c r="D28" s="3">
         <v>19</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="45">
         <v>18.96</v>
       </c>
-      <c r="F28" s="52">
+      <c r="F28" s="45">
         <v>60</v>
       </c>
-      <c r="G28" s="52">
+      <c r="G28" s="45">
         <v>120</v>
       </c>
       <c r="H28" s="5"/>
@@ -8315,13 +8314,13 @@
       <c r="D29" s="3">
         <v>22</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="45">
         <v>11.99</v>
       </c>
-      <c r="F29" s="52">
+      <c r="F29" s="45">
         <v>40</v>
       </c>
-      <c r="G29" s="52">
+      <c r="G29" s="45">
         <v>80</v>
       </c>
       <c r="H29" s="5"/>
@@ -8372,13 +8371,13 @@
       <c r="D30" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="45">
         <v>23</v>
       </c>
-      <c r="F30" s="52">
+      <c r="F30" s="45">
         <v>70</v>
       </c>
-      <c r="G30" s="52">
+      <c r="G30" s="45">
         <v>140</v>
       </c>
       <c r="H30" s="5"/>
@@ -8421,13 +8420,13 @@
       <c r="D31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="45">
         <v>13.25</v>
       </c>
-      <c r="F31" s="52">
+      <c r="F31" s="45">
         <v>55</v>
       </c>
-      <c r="G31" s="52">
+      <c r="G31" s="45">
         <v>110</v>
       </c>
       <c r="H31" s="5"/>
@@ -8470,13 +8469,13 @@
       <c r="D32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="52">
+      <c r="E32" s="45">
         <v>13.25</v>
       </c>
-      <c r="F32" s="52">
+      <c r="F32" s="45">
         <v>53</v>
       </c>
-      <c r="G32" s="52">
+      <c r="G32" s="45">
         <v>106</v>
       </c>
       <c r="H32" s="5"/>
@@ -8519,13 +8518,13 @@
       <c r="D33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="45">
         <v>15</v>
       </c>
-      <c r="F33" s="52">
+      <c r="F33" s="45">
         <v>61</v>
       </c>
-      <c r="G33" s="52">
+      <c r="G33" s="45">
         <v>122</v>
       </c>
       <c r="H33" s="5"/>
@@ -8572,13 +8571,13 @@
       <c r="D34" s="3">
         <v>22</v>
       </c>
-      <c r="E34" s="52">
+      <c r="E34" s="45">
         <v>11.193</v>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="45">
         <v>44</v>
       </c>
-      <c r="G34" s="52">
+      <c r="G34" s="45">
         <v>88</v>
       </c>
       <c r="H34" s="5"/>
@@ -8619,13 +8618,13 @@
       <c r="D35" s="3">
         <v>2</v>
       </c>
-      <c r="E35" s="52">
+      <c r="E35" s="45">
         <v>23.46</v>
       </c>
-      <c r="F35" s="52">
+      <c r="F35" s="45">
         <v>66</v>
       </c>
-      <c r="G35" s="52">
+      <c r="G35" s="45">
         <v>66</v>
       </c>
       <c r="H35" s="5"/>
@@ -8658,13 +8657,13 @@
       <c r="D36" s="3">
         <v>2</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="45">
         <v>12.3</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="45">
         <v>55</v>
       </c>
-      <c r="G36" s="52">
+      <c r="G36" s="45">
         <v>55</v>
       </c>
       <c r="H36" s="5"/>
@@ -8697,13 +8696,13 @@
       <c r="D37" s="3">
         <v>4</v>
       </c>
-      <c r="E37" s="52">
+      <c r="E37" s="45">
         <v>53.55</v>
       </c>
-      <c r="F37" s="52">
+      <c r="F37" s="45">
         <v>135</v>
       </c>
-      <c r="G37" s="52">
+      <c r="G37" s="45">
         <v>135</v>
       </c>
       <c r="H37" s="5"/>
@@ -8735,13 +8734,13 @@
       <c r="D38" s="3">
         <v>4</v>
       </c>
-      <c r="E38" s="52">
+      <c r="E38" s="45">
         <v>66.3</v>
       </c>
-      <c r="F38" s="52">
+      <c r="F38" s="45">
         <v>127</v>
       </c>
-      <c r="G38" s="52">
+      <c r="G38" s="45">
         <v>127</v>
       </c>
       <c r="H38" s="5"/>
@@ -8771,13 +8770,13 @@
       <c r="D39" s="3">
         <v>7</v>
       </c>
-      <c r="E39" s="52">
+      <c r="E39" s="45">
         <v>26.5</v>
       </c>
-      <c r="F39" s="52">
+      <c r="F39" s="45">
         <v>79</v>
       </c>
-      <c r="G39" s="52">
+      <c r="G39" s="45">
         <v>79</v>
       </c>
       <c r="H39"/>
@@ -8809,13 +8808,13 @@
       <c r="D40" s="3">
         <v>7</v>
       </c>
-      <c r="E40" s="52">
+      <c r="E40" s="45">
         <v>26.5</v>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="45">
         <v>153</v>
       </c>
-      <c r="G40" s="52">
+      <c r="G40" s="45">
         <v>153</v>
       </c>
       <c r="H40"/>
@@ -8847,13 +8846,13 @@
       <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="52">
+      <c r="E41" s="45">
         <v>85.28</v>
       </c>
-      <c r="F41" s="52">
+      <c r="F41" s="45">
         <v>220</v>
       </c>
-      <c r="G41" s="52">
+      <c r="G41" s="45">
         <v>220</v>
       </c>
       <c r="H41"/>
@@ -8885,13 +8884,13 @@
       <c r="D42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="45">
         <v>13.25</v>
       </c>
-      <c r="F42" s="52">
+      <c r="F42" s="45">
         <v>55</v>
       </c>
-      <c r="G42" s="52">
+      <c r="G42" s="45">
         <v>55</v>
       </c>
       <c r="H42"/>
@@ -8923,13 +8922,13 @@
       <c r="D43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="52">
+      <c r="E43" s="45">
         <v>13.25</v>
       </c>
-      <c r="F43" s="52">
+      <c r="F43" s="45">
         <v>64</v>
       </c>
-      <c r="G43" s="52">
+      <c r="G43" s="45">
         <v>64</v>
       </c>
       <c r="H43"/>
@@ -8961,13 +8960,13 @@
       <c r="D44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="52">
+      <c r="E44" s="45">
         <v>13.25</v>
       </c>
-      <c r="F44" s="52">
+      <c r="F44" s="45">
         <v>48</v>
       </c>
-      <c r="G44" s="52">
+      <c r="G44" s="45">
         <v>48</v>
       </c>
       <c r="H44"/>
@@ -8999,13 +8998,13 @@
       <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="52">
+      <c r="E45" s="45">
         <v>13.25</v>
       </c>
-      <c r="F45" s="52">
+      <c r="F45" s="45">
         <v>53</v>
       </c>
-      <c r="G45" s="52">
+      <c r="G45" s="45">
         <v>53</v>
       </c>
       <c r="H45"/>
@@ -9037,13 +9036,13 @@
       <c r="D46" s="3">
         <v>19</v>
       </c>
-      <c r="E46" s="52">
+      <c r="E46" s="45">
         <v>18.008099999999999</v>
       </c>
-      <c r="F46" s="52">
+      <c r="F46" s="45">
         <v>61</v>
       </c>
-      <c r="G46" s="52">
+      <c r="G46" s="45">
         <v>61</v>
       </c>
       <c r="H46"/>
@@ -9071,13 +9070,13 @@
       <c r="D47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="45">
         <v>13.5</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="45">
         <v>64</v>
       </c>
-      <c r="G47" s="52">
+      <c r="G47" s="45">
         <v>64</v>
       </c>
       <c r="H47"/>
@@ -9105,13 +9104,13 @@
       <c r="D48" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="52">
+      <c r="E48" s="45">
         <v>15</v>
       </c>
-      <c r="F48" s="52">
+      <c r="F48" s="45">
         <v>65</v>
       </c>
-      <c r="G48" s="52">
+      <c r="G48" s="45">
         <v>65</v>
       </c>
       <c r="H48"/>
@@ -9139,13 +9138,13 @@
       <c r="D49" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="52">
+      <c r="E49" s="45">
         <v>13.25</v>
       </c>
-      <c r="F49" s="52">
+      <c r="F49" s="45">
         <v>46</v>
       </c>
-      <c r="G49" s="52">
+      <c r="G49" s="45">
         <v>46</v>
       </c>
       <c r="H49"/>
@@ -9173,13 +9172,13 @@
       <c r="D50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="52">
+      <c r="E50" s="45">
         <v>13.25</v>
       </c>
-      <c r="F50" s="52">
+      <c r="F50" s="45">
         <v>51</v>
       </c>
-      <c r="G50" s="52">
+      <c r="G50" s="45">
         <v>51</v>
       </c>
       <c r="H50"/>
@@ -9264,7 +9263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2908758-2B63-4D19-8CDF-3000E5F1BE9C}">
   <dimension ref="A1:AE102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -9301,38 +9300,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="P1" s="49" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="P1" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="51"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53"/>
     </row>
     <row r="2" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -13127,787 +13126,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F5A56D-0582-46DA-B0C1-A5ABC89CFBF6}">
-  <dimension ref="A1:G64"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="D1:E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>31</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" t="b">
-        <f>A1=E1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="b">
-        <f t="shared" ref="G2:G39" si="0">A2=E2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="3">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="3">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G16" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="3">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="3">
-        <v>31</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G23" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2</v>
-      </c>
-      <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" s="3">
-        <v>2</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="3">
-        <v>15</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="3">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G29" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G30" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="3">
-        <v>26</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G31" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G32" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="3">
-        <v>21</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G33" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="3">
-        <v>8</v>
-      </c>
-      <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G35" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="G36" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="G37" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3">
-        <f>SUM(B1:B35)</f>
-        <v>219</v>
-      </c>
-      <c r="G38" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="G39" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:E35">
-    <sortCondition descending="1" ref="D1:D35"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Hopefully the last update for April's report
</commit_message>
<xml_diff>
--- a/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
+++ b/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\Output\April_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A7911-DA4D-44E2-A0C0-56B3218B878E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16AC5E1-9A4B-42D4-991F-A74E02FDC80D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="1080" windowWidth="18270" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18270" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMA Reason Codes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="186">
   <si>
     <t># of RMAs</t>
   </si>
@@ -571,22 +571,25 @@
     <t>LED-293-S00-30</t>
   </si>
   <si>
-    <t>Grand Total:</t>
-  </si>
-  <si>
     <t>BEVELED 2.0</t>
   </si>
   <si>
     <t>Totals</t>
   </si>
   <si>
-    <t>SP Kit Price</t>
-  </si>
-  <si>
-    <t>LEM Kit Price</t>
-  </si>
-  <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>SP Kit Cost</t>
+  </si>
+  <si>
+    <t>SP Price</t>
+  </si>
+  <si>
+    <t>LEM Kit Cost</t>
+  </si>
+  <si>
+    <t>LEM Price</t>
   </si>
 </sst>
 </file>
@@ -717,7 +720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -845,10 +848,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -859,21 +862,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -945,27 +939,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -975,20 +954,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -998,18 +965,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1023,6 +978,30 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5916,16 +5895,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>4761</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>23811</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>1943099</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6347,149 +6326,149 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="27">
+      <c r="K2" s="26">
         <v>109</v>
       </c>
-      <c r="L2" s="28">
+      <c r="L2" s="27">
         <f>(K2/146)*100</f>
         <v>74.657534246575338</v>
       </c>
-      <c r="N2" s="26"/>
+      <c r="N2" s="25"/>
       <c r="P2" s="9"/>
     </row>
     <row r="3" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="26">
         <v>8</v>
       </c>
-      <c r="L3" s="28">
+      <c r="L3" s="27">
         <f t="shared" ref="L3:L11" si="0">(K3/146)*100</f>
         <v>5.4794520547945202</v>
       </c>
-      <c r="N3" s="26"/>
+      <c r="N3" s="25"/>
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="26">
         <v>6</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="27">
         <f t="shared" si="0"/>
         <v>4.10958904109589</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="25"/>
       <c r="P4" s="9"/>
     </row>
     <row r="5" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
         <v>7</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="27">
         <f t="shared" si="0"/>
         <v>4.7945205479452051</v>
       </c>
-      <c r="N5" s="26"/>
+      <c r="N5" s="25"/>
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="26">
         <v>5</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <f t="shared" si="0"/>
         <v>3.4246575342465753</v>
       </c>
-      <c r="N6" s="26"/>
+      <c r="N6" s="25"/>
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="26">
         <v>4</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="27">
         <f t="shared" si="0"/>
         <v>2.7397260273972601</v>
       </c>
-      <c r="N7" s="26"/>
+      <c r="N7" s="25"/>
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="26">
         <v>3</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <f t="shared" si="0"/>
         <v>2.054794520547945</v>
       </c>
-      <c r="N8" s="26"/>
+      <c r="N8" s="25"/>
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="26">
         <v>2</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="27">
         <f t="shared" si="0"/>
         <v>1.3698630136986301</v>
       </c>
-      <c r="N9" s="26"/>
+      <c r="N9" s="25"/>
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="K10" s="27">
-        <v>1</v>
-      </c>
-      <c r="L10" s="28">
+      <c r="K10" s="26">
+        <v>1</v>
+      </c>
+      <c r="L10" s="27">
         <f t="shared" si="0"/>
         <v>0.68493150684931503</v>
       </c>
@@ -6499,17 +6478,17 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="K11" s="27">
-        <v>1</v>
-      </c>
-      <c r="L11" s="28">
+      <c r="K11" s="26">
+        <v>1</v>
+      </c>
+      <c r="L11" s="27">
         <f t="shared" si="0"/>
         <v>0.68493150684931503</v>
       </c>
-      <c r="N11" s="26"/>
+      <c r="N11" s="25"/>
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="5:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6694,8 +6673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7600A-0572-4151-919D-5CF8CE548ABA}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="K46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6704,21 +6683,21 @@
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="39" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="33" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13" style="38" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" style="38" customWidth="1"/>
-    <col min="19" max="19" width="27.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="32" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="32" customWidth="1"/>
+    <col min="19" max="19" width="27.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -6729,30 +6708,30 @@
     <col min="28" max="28" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="I1" s="5"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="32"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
       <c r="U1" s="23"/>
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
@@ -6762,54 +6741,58 @@
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
     </row>
-    <row r="2" spans="1:28" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="25" t="s">
+    <row r="2" spans="1:28" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="H2" s="5"/>
+      <c r="G2" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>181</v>
+      </c>
       <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="29" t="s">
+      <c r="L2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="Q2" s="40" t="s">
-        <v>183</v>
-      </c>
-      <c r="R2" s="40" t="s">
+      <c r="Q2" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="S2" s="33"/>
+      <c r="R2" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="S2" s="44" t="s">
+        <v>181</v>
+      </c>
       <c r="U2" s="22"/>
       <c r="V2" s="22"/>
       <c r="W2" s="22"/>
@@ -6819,54 +6802,58 @@
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
+    <row r="3" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="46">
         <v>13.25</v>
       </c>
-      <c r="F3" s="45">
-        <v>45</v>
-      </c>
-      <c r="G3" s="45">
-        <v>1350</v>
-      </c>
-      <c r="H3" s="46"/>
+      <c r="F3" s="46">
+        <v>21.3812</v>
+      </c>
+      <c r="G3" s="46">
+        <v>13.25</v>
+      </c>
+      <c r="H3" s="46">
+        <v>397.5</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="3">
+      <c r="L3" s="45">
         <v>5</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="45">
         <v>57</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="36">
+      <c r="P3" s="48">
         <v>11.7</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="48">
+        <v>12.561199999999999</v>
+      </c>
+      <c r="R3" s="48">
         <v>30</v>
       </c>
-      <c r="R3" s="36">
+      <c r="S3" s="48">
         <v>1710</v>
       </c>
-      <c r="S3" s="34"/>
       <c r="U3" s="24"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
@@ -6889,16 +6876,18 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="47">
         <v>12.3</v>
       </c>
-      <c r="F4" s="45">
-        <v>38</v>
-      </c>
-      <c r="G4" s="45">
-        <v>950</v>
-      </c>
-      <c r="H4" s="5"/>
+      <c r="F4" s="47">
+        <v>17.95</v>
+      </c>
+      <c r="G4" s="47">
+        <v>12.3</v>
+      </c>
+      <c r="H4" s="47">
+        <v>307.5</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -6918,12 +6907,14 @@
         <v>13.8</v>
       </c>
       <c r="Q4" s="36">
+        <v>15.709</v>
+      </c>
+      <c r="R4" s="36">
         <v>40</v>
       </c>
-      <c r="R4" s="36">
+      <c r="S4" s="36">
         <v>1640</v>
       </c>
-      <c r="S4" s="34"/>
       <c r="U4" s="24"/>
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
@@ -6946,16 +6937,18 @@
       <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="47">
         <v>15</v>
       </c>
-      <c r="F5" s="45">
-        <v>52</v>
-      </c>
-      <c r="G5" s="45">
-        <v>832</v>
-      </c>
-      <c r="H5" s="5"/>
+      <c r="F5" s="47">
+        <v>24</v>
+      </c>
+      <c r="G5" s="47">
+        <v>15</v>
+      </c>
+      <c r="H5" s="47">
+        <v>240</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -6975,12 +6968,14 @@
         <v>2.8355999999999999</v>
       </c>
       <c r="Q5" s="36">
+        <v>4.1326999999999998</v>
+      </c>
+      <c r="R5" s="36">
         <v>25</v>
       </c>
-      <c r="R5" s="36">
+      <c r="S5" s="36">
         <v>850</v>
       </c>
-      <c r="S5" s="34"/>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
@@ -7003,16 +6998,18 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="47">
         <v>12.67</v>
       </c>
-      <c r="F6" s="45">
-        <v>45</v>
-      </c>
-      <c r="G6" s="45">
-        <v>630</v>
-      </c>
-      <c r="H6" s="5"/>
+      <c r="F6" s="47">
+        <v>22.6</v>
+      </c>
+      <c r="G6" s="47">
+        <v>12.67</v>
+      </c>
+      <c r="H6" s="47">
+        <v>177.38</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -7032,12 +7029,14 @@
         <v>11.7</v>
       </c>
       <c r="Q6" s="36">
+        <v>13.609</v>
+      </c>
+      <c r="R6" s="36">
         <v>30</v>
       </c>
-      <c r="R6" s="36">
+      <c r="S6" s="36">
         <v>690</v>
       </c>
-      <c r="S6" s="34"/>
       <c r="U6" s="24"/>
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
@@ -7060,16 +7059,18 @@
       <c r="D7" s="3">
         <v>22</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="47">
         <v>11.99</v>
       </c>
-      <c r="F7" s="45">
-        <v>48</v>
-      </c>
-      <c r="G7" s="45">
-        <v>624</v>
-      </c>
-      <c r="H7" s="5"/>
+      <c r="F7" s="47">
+        <v>22.16</v>
+      </c>
+      <c r="G7" s="47">
+        <v>11.99</v>
+      </c>
+      <c r="H7" s="47">
+        <v>155.87</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -7089,12 +7090,14 @@
         <v>10.25</v>
       </c>
       <c r="Q7" s="36">
+        <v>11.613899999999999</v>
+      </c>
+      <c r="R7" s="36">
         <v>35</v>
       </c>
-      <c r="R7" s="36">
+      <c r="S7" s="36">
         <v>770</v>
       </c>
-      <c r="S7" s="34"/>
       <c r="U7" s="24"/>
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
@@ -7117,16 +7120,18 @@
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="47">
         <v>45.39</v>
       </c>
-      <c r="F8" s="45">
-        <v>114</v>
-      </c>
-      <c r="G8" s="45">
-        <v>1368</v>
-      </c>
-      <c r="H8" s="5"/>
+      <c r="F8" s="47">
+        <v>51.68</v>
+      </c>
+      <c r="G8" s="47">
+        <v>45.39</v>
+      </c>
+      <c r="H8" s="47">
+        <v>544.67999999999995</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -7146,12 +7151,14 @@
         <v>2.8355999999999999</v>
       </c>
       <c r="Q8" s="36">
+        <v>4.1326999999999998</v>
+      </c>
+      <c r="R8" s="36">
         <v>20</v>
       </c>
-      <c r="R8" s="36">
+      <c r="S8" s="36">
         <v>400</v>
       </c>
-      <c r="S8" s="34"/>
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
@@ -7174,16 +7181,18 @@
       <c r="D9" s="3">
         <v>19</v>
       </c>
-      <c r="E9" s="45">
+      <c r="E9" s="47">
         <v>18.9618</v>
       </c>
-      <c r="F9" s="45">
-        <v>50</v>
-      </c>
-      <c r="G9" s="45">
-        <v>600</v>
-      </c>
-      <c r="H9" s="5"/>
+      <c r="F9" s="47">
+        <v>24.712700000000002</v>
+      </c>
+      <c r="G9" s="47">
+        <v>18.9618</v>
+      </c>
+      <c r="H9" s="47">
+        <v>227.54159999999999</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -7203,12 +7212,14 @@
         <v>20.100000000000001</v>
       </c>
       <c r="Q9" s="36">
+        <v>20.725000000000001</v>
+      </c>
+      <c r="R9" s="36">
         <v>60</v>
       </c>
-      <c r="R9" s="36">
+      <c r="S9" s="36">
         <v>1020</v>
       </c>
-      <c r="S9" s="34"/>
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
@@ -7231,16 +7242,18 @@
       <c r="D10" s="3">
         <v>22</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="47">
         <v>11.986000000000001</v>
       </c>
-      <c r="F10" s="45">
-        <v>42</v>
-      </c>
-      <c r="G10" s="45">
-        <v>420</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="F10" s="47">
+        <v>21.000399999999999</v>
+      </c>
+      <c r="G10" s="47">
+        <v>11.986000000000001</v>
+      </c>
+      <c r="H10" s="47">
+        <v>119.86</v>
+      </c>
       <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -7260,12 +7273,14 @@
         <v>2.8355999999999999</v>
       </c>
       <c r="Q10" s="36">
+        <v>4.1326999999999998</v>
+      </c>
+      <c r="R10" s="36">
         <v>20</v>
       </c>
-      <c r="R10" s="36">
+      <c r="S10" s="36">
         <v>320</v>
       </c>
-      <c r="S10" s="34"/>
       <c r="U10" s="24"/>
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
@@ -7288,16 +7303,18 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="47">
         <v>14.208600000000001</v>
       </c>
-      <c r="F11" s="45">
-        <v>44</v>
-      </c>
-      <c r="G11" s="45">
-        <v>352</v>
-      </c>
-      <c r="H11" s="5"/>
+      <c r="F11" s="47">
+        <v>20.763999999999999</v>
+      </c>
+      <c r="G11" s="47">
+        <v>14.208600000000001</v>
+      </c>
+      <c r="H11" s="47">
+        <v>113.6688</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -7317,12 +7334,14 @@
         <v>11.7</v>
       </c>
       <c r="Q11" s="36">
+        <v>12.561199999999999</v>
+      </c>
+      <c r="R11" s="36">
         <v>30</v>
       </c>
-      <c r="R11" s="36">
+      <c r="S11" s="36">
         <v>330</v>
       </c>
-      <c r="S11" s="34"/>
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
@@ -7345,16 +7364,18 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="47">
         <v>12.67</v>
       </c>
-      <c r="F12" s="45">
-        <v>43</v>
-      </c>
-      <c r="G12" s="45">
-        <v>301</v>
-      </c>
-      <c r="H12" s="5"/>
+      <c r="F12" s="47">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="G12" s="47">
+        <v>12.67</v>
+      </c>
+      <c r="H12" s="47">
+        <v>88.69</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -7374,12 +7395,14 @@
         <v>11.7</v>
       </c>
       <c r="Q12" s="36">
+        <v>12.3874</v>
+      </c>
+      <c r="R12" s="36">
         <v>35</v>
       </c>
-      <c r="R12" s="36">
+      <c r="S12" s="36">
         <v>315</v>
       </c>
-      <c r="S12" s="34"/>
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
@@ -7402,16 +7425,18 @@
       <c r="D13" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="47">
         <v>40</v>
       </c>
-      <c r="F13" s="45">
-        <v>133</v>
-      </c>
-      <c r="G13" s="45">
-        <v>665</v>
-      </c>
-      <c r="H13" s="5"/>
+      <c r="F13" s="47">
+        <v>62.42</v>
+      </c>
+      <c r="G13" s="47">
+        <v>40</v>
+      </c>
+      <c r="H13" s="47">
+        <v>200</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -7431,12 +7456,14 @@
         <v>14.42</v>
       </c>
       <c r="Q13" s="36">
+        <v>15.045</v>
+      </c>
+      <c r="R13" s="36">
         <v>40</v>
       </c>
-      <c r="R13" s="36">
+      <c r="S13" s="36">
         <v>240</v>
       </c>
-      <c r="S13" s="34"/>
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
@@ -7459,16 +7486,18 @@
       <c r="D14" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="47">
         <v>35.19</v>
       </c>
-      <c r="F14" s="45">
-        <v>98</v>
-      </c>
-      <c r="G14" s="45">
-        <v>490</v>
-      </c>
-      <c r="H14" s="5"/>
+      <c r="F14" s="47">
+        <v>44.95</v>
+      </c>
+      <c r="G14" s="47">
+        <v>35.19</v>
+      </c>
+      <c r="H14" s="47">
+        <v>175.95</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -7488,12 +7517,14 @@
         <v>2.8355999999999999</v>
       </c>
       <c r="Q14" s="36">
+        <v>4.1326999999999998</v>
+      </c>
+      <c r="R14" s="36">
         <v>20</v>
       </c>
-      <c r="R14" s="36">
+      <c r="S14" s="36">
         <v>120</v>
       </c>
-      <c r="S14" s="34"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
@@ -7516,16 +7547,18 @@
       <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="47">
         <v>15.72</v>
       </c>
-      <c r="F15" s="45">
-        <v>49</v>
-      </c>
-      <c r="G15" s="45">
-        <v>196</v>
-      </c>
-      <c r="H15" s="5"/>
+      <c r="F15" s="47">
+        <v>27.37</v>
+      </c>
+      <c r="G15" s="47">
+        <v>15.72</v>
+      </c>
+      <c r="H15" s="47">
+        <v>62.88</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -7545,12 +7578,14 @@
         <v>21.5</v>
       </c>
       <c r="Q15" s="36">
+        <v>23.408999999999999</v>
+      </c>
+      <c r="R15" s="36">
         <v>75</v>
       </c>
-      <c r="R15" s="36">
+      <c r="S15" s="36">
         <v>375</v>
       </c>
-      <c r="S15" s="34"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
       <c r="W15" s="24"/>
@@ -7573,16 +7608,18 @@
       <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="47">
         <v>14.555400000000001</v>
       </c>
-      <c r="F16" s="45">
-        <v>55</v>
-      </c>
-      <c r="G16" s="45">
-        <v>220</v>
-      </c>
-      <c r="H16" s="5"/>
+      <c r="F16" s="47">
+        <v>25.419499999999999</v>
+      </c>
+      <c r="G16" s="47">
+        <v>14.555400000000001</v>
+      </c>
+      <c r="H16" s="47">
+        <v>58.221600000000002</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -7602,12 +7639,14 @@
         <v>11.7</v>
       </c>
       <c r="Q16" s="36">
+        <v>12.3874</v>
+      </c>
+      <c r="R16" s="36">
         <v>35</v>
       </c>
-      <c r="R16" s="36">
+      <c r="S16" s="36">
         <v>140</v>
       </c>
-      <c r="S16" s="34"/>
       <c r="U16" s="24"/>
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
@@ -7630,16 +7669,18 @@
       <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="47">
         <v>40</v>
       </c>
-      <c r="F17" s="45">
-        <v>112</v>
-      </c>
-      <c r="G17" s="45">
-        <v>336</v>
-      </c>
-      <c r="H17" s="5"/>
+      <c r="F17" s="47">
+        <v>53.94</v>
+      </c>
+      <c r="G17" s="47">
+        <v>40</v>
+      </c>
+      <c r="H17" s="47">
+        <v>120</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -7659,12 +7700,14 @@
         <v>11.7</v>
       </c>
       <c r="Q17" s="36">
+        <v>12.561199999999999</v>
+      </c>
+      <c r="R17" s="36">
         <v>30</v>
       </c>
-      <c r="R17" s="36">
+      <c r="S17" s="36">
         <v>120</v>
       </c>
-      <c r="S17" s="34"/>
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
@@ -7687,16 +7730,18 @@
       <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="47">
         <v>45.39</v>
       </c>
-      <c r="F18" s="45">
-        <v>117</v>
-      </c>
-      <c r="G18" s="45">
-        <v>351</v>
-      </c>
-      <c r="H18" s="5"/>
+      <c r="F18" s="47">
+        <v>52.74</v>
+      </c>
+      <c r="G18" s="47">
+        <v>45.39</v>
+      </c>
+      <c r="H18" s="47">
+        <v>136.16999999999999</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -7710,18 +7755,20 @@
         <v>172</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P18" s="36">
         <v>31.599599999999999</v>
       </c>
       <c r="Q18" s="36">
+        <v>33.480899999999998</v>
+      </c>
+      <c r="R18" s="36">
         <v>80</v>
       </c>
-      <c r="R18" s="36">
+      <c r="S18" s="36">
         <v>320</v>
       </c>
-      <c r="S18" s="34"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
@@ -7744,16 +7791,18 @@
       <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="47">
         <v>15.72</v>
       </c>
-      <c r="F19" s="45">
-        <v>46</v>
-      </c>
-      <c r="G19" s="45">
-        <v>138</v>
-      </c>
-      <c r="H19" s="5"/>
+      <c r="F19" s="47">
+        <v>21.37</v>
+      </c>
+      <c r="G19" s="47">
+        <v>15.72</v>
+      </c>
+      <c r="H19" s="47">
+        <v>47.16</v>
+      </c>
       <c r="I19" s="5"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -7773,12 +7822,14 @@
         <v>13.8</v>
       </c>
       <c r="Q19" s="36">
+        <v>15.709</v>
+      </c>
+      <c r="R19" s="36">
         <v>45</v>
       </c>
-      <c r="R19" s="36">
+      <c r="S19" s="36">
         <v>135</v>
       </c>
-      <c r="S19" s="34"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
@@ -7801,16 +7852,18 @@
       <c r="D20" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="47">
         <v>24</v>
       </c>
-      <c r="F20" s="45">
-        <v>75</v>
-      </c>
-      <c r="G20" s="45">
-        <v>225</v>
-      </c>
-      <c r="H20" s="5"/>
+      <c r="F20" s="47">
+        <v>33.689700000000002</v>
+      </c>
+      <c r="G20" s="47">
+        <v>24</v>
+      </c>
+      <c r="H20" s="47">
+        <v>72</v>
+      </c>
       <c r="I20" s="5"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -7830,12 +7883,14 @@
         <v>11.7</v>
       </c>
       <c r="Q20" s="36">
+        <v>12.561199999999999</v>
+      </c>
+      <c r="R20" s="36">
         <v>30</v>
       </c>
-      <c r="R20" s="36">
+      <c r="S20" s="36">
         <v>60</v>
       </c>
-      <c r="S20" s="34"/>
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
@@ -7858,16 +7913,18 @@
       <c r="D21" s="3">
         <v>22</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="47">
         <v>12.19</v>
       </c>
-      <c r="F21" s="45">
-        <v>39</v>
-      </c>
-      <c r="G21" s="45">
-        <v>117</v>
-      </c>
-      <c r="H21" s="5"/>
+      <c r="F21" s="47">
+        <v>20.64</v>
+      </c>
+      <c r="G21" s="47">
+        <v>12.19</v>
+      </c>
+      <c r="H21" s="47">
+        <v>36.57</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -7887,12 +7944,14 @@
         <v>14.43</v>
       </c>
       <c r="Q21" s="36">
+        <v>15.2288</v>
+      </c>
+      <c r="R21" s="36">
         <v>45</v>
       </c>
-      <c r="R21" s="36">
+      <c r="S21" s="36">
         <v>90</v>
       </c>
-      <c r="S21" s="34"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
@@ -7915,16 +7974,18 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="47">
         <v>17.649999999999999</v>
       </c>
-      <c r="F22" s="45">
-        <v>87</v>
-      </c>
-      <c r="G22" s="45">
-        <v>174</v>
-      </c>
-      <c r="H22" s="5"/>
+      <c r="F22" s="47">
+        <v>40.29</v>
+      </c>
+      <c r="G22" s="47">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="H22" s="47">
+        <v>35.299999999999997</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -7944,12 +8005,14 @@
         <v>44</v>
       </c>
       <c r="Q22" s="36">
+        <v>45.908999999999999</v>
+      </c>
+      <c r="R22" s="36">
         <v>90</v>
       </c>
-      <c r="R22" s="36">
+      <c r="S22" s="36">
         <v>180</v>
       </c>
-      <c r="S22" s="34"/>
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
       <c r="W22" s="24"/>
@@ -7972,16 +8035,18 @@
       <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="47">
         <v>45.39</v>
       </c>
-      <c r="F23" s="45">
-        <v>115</v>
-      </c>
-      <c r="G23" s="45">
-        <v>230</v>
-      </c>
-      <c r="H23" s="5"/>
+      <c r="F23" s="47">
+        <v>54.47</v>
+      </c>
+      <c r="G23" s="47">
+        <v>45.39</v>
+      </c>
+      <c r="H23" s="47">
+        <v>90.78</v>
+      </c>
       <c r="I23" s="5"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -8001,12 +8066,14 @@
         <v>27.2</v>
       </c>
       <c r="Q23" s="36">
+        <v>29.135300000000001</v>
+      </c>
+      <c r="R23" s="36">
         <v>64</v>
       </c>
-      <c r="R23" s="36">
+      <c r="S23" s="36">
         <v>128</v>
       </c>
-      <c r="S23" s="34"/>
       <c r="U23" s="24"/>
       <c r="V23" s="24"/>
       <c r="W23" s="24"/>
@@ -8029,16 +8096,18 @@
       <c r="D24" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="47">
         <v>23</v>
       </c>
-      <c r="F24" s="45">
-        <v>79</v>
-      </c>
-      <c r="G24" s="45">
-        <v>158</v>
-      </c>
-      <c r="H24" s="5"/>
+      <c r="F24" s="47">
+        <v>36.7211</v>
+      </c>
+      <c r="G24" s="47">
+        <v>23</v>
+      </c>
+      <c r="H24" s="47">
+        <v>46</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -8058,12 +8127,14 @@
         <v>25.3</v>
       </c>
       <c r="Q24" s="36">
+        <v>25.925000000000001</v>
+      </c>
+      <c r="R24" s="36">
         <v>56</v>
       </c>
-      <c r="R24" s="36">
+      <c r="S24" s="36">
         <v>112</v>
       </c>
-      <c r="S24" s="34"/>
       <c r="U24" s="24"/>
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
@@ -8086,16 +8157,18 @@
       <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="45">
+      <c r="E25" s="47">
         <v>15.72</v>
       </c>
-      <c r="F25" s="45">
-        <v>39</v>
-      </c>
-      <c r="G25" s="45">
-        <v>78</v>
-      </c>
-      <c r="H25" s="5"/>
+      <c r="F25" s="47">
+        <v>23.88</v>
+      </c>
+      <c r="G25" s="47">
+        <v>15.72</v>
+      </c>
+      <c r="H25" s="47">
+        <v>31.44</v>
+      </c>
       <c r="I25" s="5"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -8115,12 +8188,14 @@
         <v>15.6813</v>
       </c>
       <c r="Q25" s="36">
+        <v>15.6813</v>
+      </c>
+      <c r="R25" s="36">
         <v>40</v>
       </c>
-      <c r="R25" s="36">
+      <c r="S25" s="36">
         <v>80</v>
       </c>
-      <c r="S25" s="34"/>
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
@@ -8143,16 +8218,18 @@
       <c r="D26" s="3">
         <v>2</v>
       </c>
-      <c r="E26" s="45">
+      <c r="E26" s="47">
         <v>14.31</v>
       </c>
-      <c r="F26" s="45">
-        <v>52</v>
-      </c>
-      <c r="G26" s="45">
-        <v>104</v>
-      </c>
-      <c r="H26" s="5"/>
+      <c r="F26" s="47">
+        <v>23.09</v>
+      </c>
+      <c r="G26" s="47">
+        <v>14.31</v>
+      </c>
+      <c r="H26" s="47">
+        <v>28.62</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -8172,12 +8249,14 @@
         <v>30.98</v>
       </c>
       <c r="Q26" s="36">
-        <v>75</v>
+        <v>32.889000000000003</v>
       </c>
       <c r="R26" s="36">
         <v>75</v>
       </c>
-      <c r="S26" s="34"/>
+      <c r="S26" s="36">
+        <v>75</v>
+      </c>
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
@@ -8200,16 +8279,18 @@
       <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="E27" s="45">
+      <c r="E27" s="47">
         <v>14.31</v>
       </c>
-      <c r="F27" s="45">
-        <v>54</v>
-      </c>
-      <c r="G27" s="45">
-        <v>108</v>
-      </c>
-      <c r="H27" s="5"/>
+      <c r="F27" s="47">
+        <v>23.49</v>
+      </c>
+      <c r="G27" s="47">
+        <v>14.31</v>
+      </c>
+      <c r="H27" s="47">
+        <v>28.62</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -8229,12 +8310,14 @@
         <v>11.7</v>
       </c>
       <c r="Q27" s="36">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="R27" s="36">
         <v>30</v>
       </c>
-      <c r="S27" s="34"/>
+      <c r="S27" s="36">
+        <v>30</v>
+      </c>
       <c r="U27" s="24"/>
       <c r="V27" s="24"/>
       <c r="W27" s="24"/>
@@ -8257,16 +8340,18 @@
       <c r="D28" s="3">
         <v>19</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="47">
         <v>18.96</v>
       </c>
-      <c r="F28" s="45">
-        <v>60</v>
-      </c>
-      <c r="G28" s="45">
-        <v>120</v>
-      </c>
-      <c r="H28" s="5"/>
+      <c r="F28" s="47">
+        <v>31.58</v>
+      </c>
+      <c r="G28" s="47">
+        <v>18.96</v>
+      </c>
+      <c r="H28" s="47">
+        <v>37.92</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -8286,12 +8371,14 @@
         <v>11.7</v>
       </c>
       <c r="Q28" s="36">
-        <v>30</v>
+        <v>13.609</v>
       </c>
       <c r="R28" s="36">
         <v>30</v>
       </c>
-      <c r="S28" s="34"/>
+      <c r="S28" s="36">
+        <v>30</v>
+      </c>
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
       <c r="W28" s="24"/>
@@ -8314,16 +8401,18 @@
       <c r="D29" s="3">
         <v>22</v>
       </c>
-      <c r="E29" s="45">
+      <c r="E29" s="47">
         <v>11.99</v>
       </c>
-      <c r="F29" s="45">
-        <v>40</v>
-      </c>
-      <c r="G29" s="45">
-        <v>80</v>
-      </c>
-      <c r="H29" s="5"/>
+      <c r="F29" s="47">
+        <v>20.43</v>
+      </c>
+      <c r="G29" s="47">
+        <v>11.99</v>
+      </c>
+      <c r="H29" s="47">
+        <v>23.98</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -8343,12 +8432,14 @@
         <v>39.85</v>
       </c>
       <c r="Q29" s="36">
-        <v>90</v>
+        <v>42.3491</v>
       </c>
       <c r="R29" s="36">
         <v>90</v>
       </c>
-      <c r="S29" s="34"/>
+      <c r="S29" s="36">
+        <v>90</v>
+      </c>
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
@@ -8371,16 +8462,18 @@
       <c r="D30" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E30" s="45">
+      <c r="E30" s="47">
         <v>23</v>
       </c>
-      <c r="F30" s="45">
-        <v>70</v>
-      </c>
-      <c r="G30" s="45">
-        <v>140</v>
-      </c>
-      <c r="H30" s="5"/>
+      <c r="F30" s="47">
+        <v>32.69</v>
+      </c>
+      <c r="G30" s="47">
+        <v>23</v>
+      </c>
+      <c r="H30" s="47">
+        <v>46</v>
+      </c>
       <c r="I30" s="5"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -8400,12 +8493,14 @@
         <v>13.8</v>
       </c>
       <c r="Q30" s="36">
-        <v>40</v>
+        <v>15.709</v>
       </c>
       <c r="R30" s="36">
         <v>40</v>
       </c>
-      <c r="S30" s="34"/>
+      <c r="S30" s="36">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -8420,16 +8515,18 @@
       <c r="D31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="47">
         <v>13.25</v>
       </c>
-      <c r="F31" s="45">
-        <v>55</v>
-      </c>
-      <c r="G31" s="45">
-        <v>110</v>
-      </c>
-      <c r="H31" s="5"/>
+      <c r="F31" s="47">
+        <v>26.34</v>
+      </c>
+      <c r="G31" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H31" s="47">
+        <v>26.5</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -8449,12 +8546,14 @@
         <v>23.95</v>
       </c>
       <c r="Q31" s="36">
-        <v>65</v>
+        <v>25.859000000000002</v>
       </c>
       <c r="R31" s="36">
         <v>65</v>
       </c>
-      <c r="S31" s="34"/>
+      <c r="S31" s="36">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -8469,16 +8568,18 @@
       <c r="D32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="47">
         <v>13.25</v>
       </c>
-      <c r="F32" s="45">
-        <v>53</v>
-      </c>
-      <c r="G32" s="45">
-        <v>106</v>
-      </c>
-      <c r="H32" s="5"/>
+      <c r="F32" s="47">
+        <v>23.35</v>
+      </c>
+      <c r="G32" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H32" s="47">
+        <v>26.5</v>
+      </c>
       <c r="I32" s="5"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -8498,12 +8599,14 @@
         <v>10.55</v>
       </c>
       <c r="Q32" s="36">
-        <v>40</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="R32" s="36">
         <v>40</v>
       </c>
-      <c r="S32" s="34"/>
+      <c r="S32" s="36">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -8518,16 +8621,18 @@
       <c r="D33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="47">
         <v>15</v>
       </c>
-      <c r="F33" s="45">
-        <v>61</v>
-      </c>
-      <c r="G33" s="45">
-        <v>122</v>
-      </c>
-      <c r="H33" s="5"/>
+      <c r="F33" s="47">
+        <v>28.15</v>
+      </c>
+      <c r="G33" s="47">
+        <v>15</v>
+      </c>
+      <c r="H33" s="47">
+        <v>30</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -8547,12 +8652,14 @@
         <v>10.25</v>
       </c>
       <c r="Q33" s="36">
-        <v>35</v>
+        <v>11.613899999999999</v>
       </c>
       <c r="R33" s="36">
         <v>35</v>
       </c>
-      <c r="S33" s="34"/>
+      <c r="S33" s="36">
+        <v>35</v>
+      </c>
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
       <c r="Y33" s="24"/>
@@ -8571,35 +8678,29 @@
       <c r="D34" s="3">
         <v>22</v>
       </c>
-      <c r="E34" s="45">
+      <c r="E34" s="47">
         <v>11.193</v>
       </c>
-      <c r="F34" s="45">
-        <v>44</v>
-      </c>
-      <c r="G34" s="45">
-        <v>88</v>
-      </c>
-      <c r="H34" s="5"/>
+      <c r="F34" s="47">
+        <v>19.637499999999999</v>
+      </c>
+      <c r="G34" s="47">
+        <v>11.193</v>
+      </c>
+      <c r="H34" s="47">
+        <v>22.385999999999999</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30">
-        <f>SUM(M3:M33)</f>
-        <v>302</v>
-      </c>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="R34" s="36">
-        <f>SUM(R3:R33)</f>
-        <v>10550</v>
-      </c>
-      <c r="S34" s="34"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="34"/>
+      <c r="S34" s="29"/>
       <c r="W34" s="24"/>
       <c r="X34" s="24"/>
       <c r="Y34" s="24"/>
@@ -8618,16 +8719,18 @@
       <c r="D35" s="3">
         <v>2</v>
       </c>
-      <c r="E35" s="45">
+      <c r="E35" s="47">
         <v>23.46</v>
       </c>
-      <c r="F35" s="45">
-        <v>66</v>
-      </c>
-      <c r="G35" s="45">
-        <v>66</v>
-      </c>
-      <c r="H35" s="5"/>
+      <c r="F35" s="47">
+        <v>31.468399999999999</v>
+      </c>
+      <c r="G35" s="47">
+        <v>23.46</v>
+      </c>
+      <c r="H35" s="47">
+        <v>23.46</v>
+      </c>
       <c r="I35" s="5"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -8635,10 +8738,10 @@
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="34"/>
+      <c r="P35" s="34"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="29"/>
       <c r="W35" s="24"/>
       <c r="X35" s="24"/>
       <c r="Y35" s="24"/>
@@ -8657,16 +8760,18 @@
       <c r="D36" s="3">
         <v>2</v>
       </c>
-      <c r="E36" s="45">
+      <c r="E36" s="47">
         <v>12.3</v>
       </c>
-      <c r="F36" s="45">
-        <v>55</v>
-      </c>
-      <c r="G36" s="45">
-        <v>55</v>
-      </c>
-      <c r="H36" s="5"/>
+      <c r="F36" s="47">
+        <v>24.4</v>
+      </c>
+      <c r="G36" s="47">
+        <v>12.3</v>
+      </c>
+      <c r="H36" s="47">
+        <v>12.3</v>
+      </c>
       <c r="I36" s="5"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -8674,10 +8779,10 @@
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
-      <c r="P36" s="43"/>
-      <c r="Q36" s="43"/>
-      <c r="R36" s="43"/>
-      <c r="S36" s="34"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="29"/>
       <c r="W36" s="24"/>
       <c r="X36" s="24"/>
       <c r="Y36" s="24"/>
@@ -8696,16 +8801,18 @@
       <c r="D37" s="3">
         <v>4</v>
       </c>
-      <c r="E37" s="45">
+      <c r="E37" s="47">
         <v>53.55</v>
       </c>
-      <c r="F37" s="45">
-        <v>135</v>
-      </c>
-      <c r="G37" s="45">
-        <v>135</v>
-      </c>
-      <c r="H37" s="5"/>
+      <c r="F37" s="47">
+        <v>60.65</v>
+      </c>
+      <c r="G37" s="47">
+        <v>53.55</v>
+      </c>
+      <c r="H37" s="47">
+        <v>53.55</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -8713,9 +8820,9 @@
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="43"/>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="43"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="34"/>
       <c r="W37" s="24"/>
       <c r="X37" s="24"/>
       <c r="Y37" s="24"/>
@@ -8734,16 +8841,18 @@
       <c r="D38" s="3">
         <v>4</v>
       </c>
-      <c r="E38" s="45">
+      <c r="E38" s="47">
         <v>66.3</v>
       </c>
-      <c r="F38" s="45">
-        <v>127</v>
-      </c>
-      <c r="G38" s="45">
-        <v>127</v>
-      </c>
-      <c r="H38" s="5"/>
+      <c r="F38" s="47">
+        <v>73.319999999999993</v>
+      </c>
+      <c r="G38" s="47">
+        <v>66.3</v>
+      </c>
+      <c r="H38" s="47">
+        <v>66.3</v>
+      </c>
       <c r="I38" s="5"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -8751,7 +8860,7 @@
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="5"/>
-      <c r="P38" s="43"/>
+      <c r="P38" s="34"/>
       <c r="W38" s="24"/>
       <c r="X38" s="24"/>
       <c r="Y38" s="24"/>
@@ -8770,26 +8879,28 @@
       <c r="D39" s="3">
         <v>7</v>
       </c>
-      <c r="E39" s="45">
+      <c r="E39" s="47">
         <v>26.5</v>
       </c>
-      <c r="F39" s="45">
-        <v>79</v>
-      </c>
-      <c r="G39" s="45">
-        <v>79</v>
-      </c>
-      <c r="H39"/>
+      <c r="F39" s="47">
+        <v>36.1496</v>
+      </c>
+      <c r="G39" s="47">
+        <v>26.5</v>
+      </c>
+      <c r="H39" s="47">
+        <v>26.5</v>
+      </c>
       <c r="I39"/>
       <c r="O39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P39" s="36">
+      <c r="P39" s="31">
         <v>57</v>
       </c>
-      <c r="Q39" s="43"/>
-      <c r="R39" s="43"/>
-      <c r="S39" s="35"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="30"/>
       <c r="W39" s="24"/>
       <c r="X39" s="24"/>
       <c r="Y39" s="24"/>
@@ -8808,26 +8919,28 @@
       <c r="D40" s="3">
         <v>7</v>
       </c>
-      <c r="E40" s="45">
+      <c r="E40" s="47">
         <v>26.5</v>
       </c>
-      <c r="F40" s="45">
-        <v>153</v>
-      </c>
-      <c r="G40" s="45">
-        <v>153</v>
-      </c>
-      <c r="H40"/>
+      <c r="F40" s="47">
+        <v>50.839300000000001</v>
+      </c>
+      <c r="G40" s="47">
+        <v>26.5</v>
+      </c>
+      <c r="H40" s="47">
+        <v>26.5</v>
+      </c>
       <c r="I40"/>
       <c r="O40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="36">
+      <c r="P40" s="31">
         <v>41</v>
       </c>
-      <c r="Q40" s="43"/>
-      <c r="R40" s="43"/>
-      <c r="S40" s="35"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="30"/>
       <c r="W40" s="24"/>
       <c r="X40" s="24"/>
       <c r="Y40" s="24"/>
@@ -8846,26 +8959,28 @@
       <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="45">
+      <c r="E41" s="47">
         <v>85.28</v>
       </c>
-      <c r="F41" s="45">
-        <v>220</v>
-      </c>
-      <c r="G41" s="45">
-        <v>220</v>
-      </c>
-      <c r="H41"/>
+      <c r="F41" s="47">
+        <v>93.844999999999999</v>
+      </c>
+      <c r="G41" s="47">
+        <v>85.28</v>
+      </c>
+      <c r="H41" s="47">
+        <v>85.28</v>
+      </c>
       <c r="I41"/>
       <c r="O41" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="P41" s="36">
+      <c r="P41" s="31">
         <v>34</v>
       </c>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="35"/>
+      <c r="Q41" s="34"/>
+      <c r="R41" s="34"/>
+      <c r="S41" s="30"/>
       <c r="W41" s="24"/>
       <c r="X41" s="24"/>
       <c r="Y41" s="24"/>
@@ -8884,26 +8999,28 @@
       <c r="D42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="45">
+      <c r="E42" s="47">
         <v>13.25</v>
       </c>
-      <c r="F42" s="45">
-        <v>55</v>
-      </c>
-      <c r="G42" s="45">
-        <v>55</v>
-      </c>
-      <c r="H42"/>
+      <c r="F42" s="47">
+        <v>24.41</v>
+      </c>
+      <c r="G42" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H42" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I42"/>
       <c r="O42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P42" s="36">
+      <c r="P42" s="31">
         <v>23</v>
       </c>
-      <c r="Q42" s="43"/>
-      <c r="R42" s="43"/>
-      <c r="S42" s="35"/>
+      <c r="Q42" s="34"/>
+      <c r="R42" s="34"/>
+      <c r="S42" s="30"/>
       <c r="W42" s="24"/>
       <c r="X42" s="24"/>
       <c r="Y42" s="24"/>
@@ -8922,26 +9039,28 @@
       <c r="D43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="45">
+      <c r="E43" s="47">
         <v>13.25</v>
       </c>
-      <c r="F43" s="45">
-        <v>64</v>
-      </c>
-      <c r="G43" s="45">
-        <v>64</v>
-      </c>
-      <c r="H43"/>
+      <c r="F43" s="47">
+        <v>22.82</v>
+      </c>
+      <c r="G43" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H43" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I43"/>
       <c r="O43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P43" s="36">
+      <c r="P43" s="31">
         <v>22</v>
       </c>
-      <c r="Q43" s="43"/>
-      <c r="R43" s="43"/>
-      <c r="S43" s="35"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="30"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -8960,26 +9079,28 @@
       <c r="D44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="45">
+      <c r="E44" s="47">
         <v>13.25</v>
       </c>
-      <c r="F44" s="45">
-        <v>48</v>
-      </c>
-      <c r="G44" s="45">
-        <v>48</v>
-      </c>
-      <c r="H44"/>
+      <c r="F44" s="47">
+        <v>22.2879</v>
+      </c>
+      <c r="G44" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H44" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I44"/>
       <c r="O44" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P44" s="36">
+      <c r="P44" s="31">
         <v>20</v>
       </c>
-      <c r="Q44" s="43"/>
-      <c r="R44" s="43"/>
-      <c r="S44" s="35"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="34"/>
+      <c r="S44" s="30"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -8998,26 +9119,28 @@
       <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="45">
+      <c r="E45" s="47">
         <v>13.25</v>
       </c>
-      <c r="F45" s="45">
-        <v>53</v>
-      </c>
-      <c r="G45" s="45">
-        <v>53</v>
-      </c>
-      <c r="H45"/>
+      <c r="F45" s="47">
+        <v>21.477699999999999</v>
+      </c>
+      <c r="G45" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H45" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I45"/>
       <c r="O45" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="P45" s="36">
+      <c r="P45" s="31">
         <v>17</v>
       </c>
-      <c r="Q45" s="43"/>
-      <c r="R45" s="43"/>
-      <c r="S45" s="35"/>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="34"/>
+      <c r="S45" s="30"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
@@ -9036,26 +9159,28 @@
       <c r="D46" s="3">
         <v>19</v>
       </c>
-      <c r="E46" s="45">
+      <c r="E46" s="47">
         <v>18.008099999999999</v>
       </c>
-      <c r="F46" s="45">
-        <v>61</v>
-      </c>
-      <c r="G46" s="45">
-        <v>61</v>
-      </c>
-      <c r="H46"/>
+      <c r="F46" s="47">
+        <v>27.285699999999999</v>
+      </c>
+      <c r="G46" s="47">
+        <v>18.008099999999999</v>
+      </c>
+      <c r="H46" s="47">
+        <v>18.008099999999999</v>
+      </c>
       <c r="I46"/>
       <c r="O46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P46" s="36">
+      <c r="P46" s="31">
         <v>16</v>
       </c>
-      <c r="Q46" s="43"/>
-      <c r="R46" s="43"/>
-      <c r="S46" s="35"/>
+      <c r="Q46" s="34"/>
+      <c r="R46" s="34"/>
+      <c r="S46" s="30"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -9070,26 +9195,28 @@
       <c r="D47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="45">
+      <c r="E47" s="47">
         <v>13.5</v>
       </c>
-      <c r="F47" s="45">
-        <v>64</v>
-      </c>
-      <c r="G47" s="45">
-        <v>64</v>
-      </c>
-      <c r="H47"/>
+      <c r="F47" s="47">
+        <v>29.4359</v>
+      </c>
+      <c r="G47" s="47">
+        <v>13.5</v>
+      </c>
+      <c r="H47" s="47">
+        <v>13.5</v>
+      </c>
       <c r="I47"/>
       <c r="O47" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="P47" s="36">
+      <c r="P47" s="31">
         <v>11</v>
       </c>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="43"/>
-      <c r="S47" s="35"/>
+      <c r="Q47" s="34"/>
+      <c r="R47" s="34"/>
+      <c r="S47" s="30"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
@@ -9104,26 +9231,28 @@
       <c r="D48" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="45">
+      <c r="E48" s="47">
         <v>15</v>
       </c>
-      <c r="F48" s="45">
-        <v>65</v>
-      </c>
-      <c r="G48" s="45">
-        <v>65</v>
-      </c>
-      <c r="H48"/>
+      <c r="F48" s="47">
+        <v>27.61</v>
+      </c>
+      <c r="G48" s="47">
+        <v>15</v>
+      </c>
+      <c r="H48" s="47">
+        <v>15</v>
+      </c>
       <c r="I48"/>
       <c r="O48" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P48" s="36">
+      <c r="P48" s="31">
         <v>9</v>
       </c>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="43"/>
-      <c r="S48" s="35"/>
+      <c r="Q48" s="34"/>
+      <c r="R48" s="34"/>
+      <c r="S48" s="30"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
@@ -9138,26 +9267,28 @@
       <c r="D49" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="45">
+      <c r="E49" s="47">
         <v>13.25</v>
       </c>
-      <c r="F49" s="45">
-        <v>46</v>
-      </c>
-      <c r="G49" s="45">
-        <v>46</v>
-      </c>
-      <c r="H49"/>
+      <c r="F49" s="47">
+        <v>22.72</v>
+      </c>
+      <c r="G49" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H49" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I49"/>
       <c r="O49" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="P49" s="36">
+      <c r="P49" s="31">
         <v>6</v>
       </c>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="43"/>
-      <c r="S49" s="35"/>
+      <c r="Q49" s="34"/>
+      <c r="R49" s="34"/>
+      <c r="S49" s="30"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
@@ -9172,26 +9303,28 @@
       <c r="D50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="45">
+      <c r="E50" s="47">
         <v>13.25</v>
       </c>
-      <c r="F50" s="45">
-        <v>51</v>
-      </c>
-      <c r="G50" s="45">
-        <v>51</v>
-      </c>
-      <c r="H50"/>
+      <c r="F50" s="47">
+        <v>23.35</v>
+      </c>
+      <c r="G50" s="47">
+        <v>13.25</v>
+      </c>
+      <c r="H50" s="47">
+        <v>13.25</v>
+      </c>
       <c r="I50"/>
       <c r="O50" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="P50" s="36">
+      <c r="P50" s="31">
         <v>6</v>
       </c>
-      <c r="Q50" s="43"/>
-      <c r="R50" s="43"/>
-      <c r="S50" s="35"/>
+      <c r="Q50" s="34"/>
+      <c r="R50" s="34"/>
+      <c r="S50" s="30"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H51"/>
@@ -9199,12 +9332,12 @@
       <c r="O51" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P51" s="36">
+      <c r="P51" s="31">
         <v>5</v>
       </c>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="43"/>
-      <c r="S51" s="35"/>
+      <c r="Q51" s="34"/>
+      <c r="R51" s="34"/>
+      <c r="S51" s="30"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H52"/>
@@ -9212,12 +9345,12 @@
       <c r="O52" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P52" s="36">
+      <c r="P52" s="31">
         <v>4</v>
       </c>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="43"/>
-      <c r="S52" s="35"/>
+      <c r="Q52" s="34"/>
+      <c r="R52" s="34"/>
+      <c r="S52" s="30"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H53"/>
@@ -9225,18 +9358,18 @@
       <c r="O53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P53" s="36">
+      <c r="P53" s="31">
         <v>4</v>
       </c>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="35"/>
+      <c r="Q53" s="34"/>
+      <c r="R53" s="34"/>
+      <c r="S53" s="30"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H54"/>
       <c r="I54"/>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="43"/>
+      <c r="Q54" s="34"/>
+      <c r="R54" s="34"/>
     </row>
     <row r="70" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J70" s="2"/>
@@ -9246,8 +9379,8 @@
     <sortCondition descending="1" ref="B3:B50"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="L1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9300,80 +9433,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="P1" s="51" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="P1" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="53"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="40"/>
     </row>
     <row r="2" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="28" t="s">
         <v>35</v>
       </c>
       <c r="P2" s="19" t="s">
@@ -12776,7 +12909,7 @@
         <v>7</v>
       </c>
       <c r="P61" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q61" s="16">
         <f>SUM(Q3:Q60)</f>
@@ -12954,7 +13087,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="16">
         <f>SUM(B3:B66)</f>

</xml_diff>

<commit_message>
Fixed price and cost columns
</commit_message>
<xml_diff>
--- a/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
+++ b/Code/Output/April_2021/Metrics_Report_April_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\Code\Output\April_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16AC5E1-9A4B-42D4-991F-A74E02FDC80D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4463E3-D672-4FE8-8942-39B4EA523D61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="18270" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="1170" windowWidth="18270" windowHeight="13695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMA Reason Codes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="184">
   <si>
     <t># of RMAs</t>
   </si>
@@ -583,13 +583,7 @@
     <t>SP Kit Cost</t>
   </si>
   <si>
-    <t>SP Price</t>
-  </si>
-  <si>
     <t>LEM Kit Cost</t>
-  </si>
-  <si>
-    <t>LEM Price</t>
   </si>
 </sst>
 </file>
@@ -720,7 +714,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -862,12 +856,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -967,24 +970,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,6 +986,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6673,8 +6688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B7600A-0572-4151-919D-5CF8CE548ABA}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="K46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6709,29 +6724,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="5"/>
       <c r="U1" s="23"/>
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
@@ -6742,57 +6757,53 @@
       <c r="AB1" s="23"/>
     </row>
     <row r="2" spans="1:28" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="43" t="s">
+      <c r="A2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" s="44" t="s">
+      <c r="G2" s="38" t="s">
         <v>181</v>
       </c>
+      <c r="H2" s="51"/>
       <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="43" t="s">
+      <c r="L2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="P2" s="44" t="s">
+      <c r="P2" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="Q2" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="R2" s="44" t="s">
-        <v>185</v>
-      </c>
-      <c r="S2" s="44" t="s">
+      <c r="Q2" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" s="38" t="s">
         <v>181</v>
       </c>
+      <c r="S2" s="51"/>
       <c r="U2" s="22"/>
       <c r="V2" s="22"/>
       <c r="W2" s="22"/>
@@ -6803,57 +6814,55 @@
       <c r="AB2" s="22"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
-        <v>1</v>
-      </c>
-      <c r="B3" s="45">
+      <c r="A3" s="39">
+        <v>1</v>
+      </c>
+      <c r="B3" s="39">
         <v>30</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="40">
         <v>13.25</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="40">
         <v>21.3812</v>
       </c>
-      <c r="G3" s="46">
-        <v>13.25</v>
-      </c>
-      <c r="H3" s="46">
-        <v>397.5</v>
-      </c>
+      <c r="G3" s="40">
+        <f>B3*F3</f>
+        <v>641.43600000000004</v>
+      </c>
+      <c r="H3" s="50"/>
       <c r="I3" s="5"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="45">
+      <c r="L3" s="39">
         <v>5</v>
       </c>
-      <c r="M3" s="45">
+      <c r="M3" s="39">
         <v>57</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="42">
         <v>11.7</v>
       </c>
-      <c r="Q3" s="48">
+      <c r="Q3" s="42">
         <v>12.561199999999999</v>
       </c>
-      <c r="R3" s="48">
-        <v>30</v>
-      </c>
-      <c r="S3" s="48">
-        <v>1710</v>
-      </c>
+      <c r="R3" s="42">
+        <f>M3*Q3</f>
+        <v>715.98839999999996</v>
+      </c>
+      <c r="S3" s="52"/>
       <c r="U3" s="24"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
@@ -6876,18 +6885,17 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="41">
         <v>12.3</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="41">
         <v>17.95</v>
       </c>
-      <c r="G4" s="47">
-        <v>12.3</v>
-      </c>
-      <c r="H4" s="47">
-        <v>307.5</v>
-      </c>
+      <c r="G4" s="41">
+        <f t="shared" ref="G4:G50" si="0">B4*F4</f>
+        <v>448.75</v>
+      </c>
+      <c r="H4" s="50"/>
       <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -6910,11 +6918,10 @@
         <v>15.709</v>
       </c>
       <c r="R4" s="36">
-        <v>40</v>
-      </c>
-      <c r="S4" s="36">
-        <v>1640</v>
-      </c>
+        <f t="shared" ref="R4:R33" si="1">M4*Q4</f>
+        <v>644.06899999999996</v>
+      </c>
+      <c r="S4" s="52"/>
       <c r="U4" s="24"/>
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
@@ -6937,18 +6944,17 @@
       <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="41">
         <v>15</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="41">
         <v>24</v>
       </c>
-      <c r="G5" s="47">
-        <v>15</v>
-      </c>
-      <c r="H5" s="47">
-        <v>240</v>
-      </c>
+      <c r="G5" s="41">
+        <f t="shared" si="0"/>
+        <v>384</v>
+      </c>
+      <c r="H5" s="50"/>
       <c r="I5" s="5"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -6971,11 +6977,10 @@
         <v>4.1326999999999998</v>
       </c>
       <c r="R5" s="36">
-        <v>25</v>
-      </c>
-      <c r="S5" s="36">
-        <v>850</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>140.51179999999999</v>
+      </c>
+      <c r="S5" s="52"/>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
@@ -6998,18 +7003,17 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="41">
         <v>12.67</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="41">
         <v>22.6</v>
       </c>
-      <c r="G6" s="47">
-        <v>12.67</v>
-      </c>
-      <c r="H6" s="47">
-        <v>177.38</v>
-      </c>
+      <c r="G6" s="41">
+        <f t="shared" si="0"/>
+        <v>316.40000000000003</v>
+      </c>
+      <c r="H6" s="50"/>
       <c r="I6" s="5"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -7032,11 +7036,10 @@
         <v>13.609</v>
       </c>
       <c r="R6" s="36">
-        <v>30</v>
-      </c>
-      <c r="S6" s="36">
-        <v>690</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>313.00700000000001</v>
+      </c>
+      <c r="S6" s="52"/>
       <c r="U6" s="24"/>
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
@@ -7059,18 +7062,17 @@
       <c r="D7" s="3">
         <v>22</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="41">
         <v>11.99</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="41">
         <v>22.16</v>
       </c>
-      <c r="G7" s="47">
-        <v>11.99</v>
-      </c>
-      <c r="H7" s="47">
-        <v>155.87</v>
-      </c>
+      <c r="G7" s="41">
+        <f t="shared" si="0"/>
+        <v>288.08</v>
+      </c>
+      <c r="H7" s="50"/>
       <c r="I7" s="5"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -7093,11 +7095,10 @@
         <v>11.613899999999999</v>
       </c>
       <c r="R7" s="36">
-        <v>35</v>
-      </c>
-      <c r="S7" s="36">
-        <v>770</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>255.50579999999999</v>
+      </c>
+      <c r="S7" s="52"/>
       <c r="U7" s="24"/>
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
@@ -7120,18 +7121,17 @@
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="41">
         <v>45.39</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="41">
         <v>51.68</v>
       </c>
-      <c r="G8" s="47">
-        <v>45.39</v>
-      </c>
-      <c r="H8" s="47">
-        <v>544.67999999999995</v>
-      </c>
+      <c r="G8" s="41">
+        <f t="shared" si="0"/>
+        <v>620.16</v>
+      </c>
+      <c r="H8" s="50"/>
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -7154,11 +7154,10 @@
         <v>4.1326999999999998</v>
       </c>
       <c r="R8" s="36">
-        <v>20</v>
-      </c>
-      <c r="S8" s="36">
-        <v>400</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>82.653999999999996</v>
+      </c>
+      <c r="S8" s="52"/>
       <c r="U8" s="24"/>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
@@ -7181,18 +7180,17 @@
       <c r="D9" s="3">
         <v>19</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="41">
         <v>18.9618</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="41">
         <v>24.712700000000002</v>
       </c>
-      <c r="G9" s="47">
-        <v>18.9618</v>
-      </c>
-      <c r="H9" s="47">
-        <v>227.54159999999999</v>
-      </c>
+      <c r="G9" s="41">
+        <f t="shared" si="0"/>
+        <v>296.55240000000003</v>
+      </c>
+      <c r="H9" s="50"/>
       <c r="I9" s="5"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -7215,11 +7213,10 @@
         <v>20.725000000000001</v>
       </c>
       <c r="R9" s="36">
-        <v>60</v>
-      </c>
-      <c r="S9" s="36">
-        <v>1020</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>352.32500000000005</v>
+      </c>
+      <c r="S9" s="52"/>
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
@@ -7242,18 +7239,17 @@
       <c r="D10" s="3">
         <v>22</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="41">
         <v>11.986000000000001</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="41">
         <v>21.000399999999999</v>
       </c>
-      <c r="G10" s="47">
-        <v>11.986000000000001</v>
-      </c>
-      <c r="H10" s="47">
-        <v>119.86</v>
-      </c>
+      <c r="G10" s="41">
+        <f t="shared" si="0"/>
+        <v>210.00399999999999</v>
+      </c>
+      <c r="H10" s="50"/>
       <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -7276,11 +7272,10 @@
         <v>4.1326999999999998</v>
       </c>
       <c r="R10" s="36">
-        <v>20</v>
-      </c>
-      <c r="S10" s="36">
-        <v>320</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>66.123199999999997</v>
+      </c>
+      <c r="S10" s="52"/>
       <c r="U10" s="24"/>
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
@@ -7303,18 +7298,17 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="41">
         <v>14.208600000000001</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="41">
         <v>20.763999999999999</v>
       </c>
-      <c r="G11" s="47">
-        <v>14.208600000000001</v>
-      </c>
-      <c r="H11" s="47">
-        <v>113.6688</v>
-      </c>
+      <c r="G11" s="41">
+        <f t="shared" si="0"/>
+        <v>166.11199999999999</v>
+      </c>
+      <c r="H11" s="50"/>
       <c r="I11" s="5"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -7337,11 +7331,10 @@
         <v>12.561199999999999</v>
       </c>
       <c r="R11" s="36">
-        <v>30</v>
-      </c>
-      <c r="S11" s="36">
-        <v>330</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>138.17320000000001</v>
+      </c>
+      <c r="S11" s="52"/>
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
@@ -7364,18 +7357,17 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="41">
         <v>12.67</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="41">
         <v>19.239999999999998</v>
       </c>
-      <c r="G12" s="47">
-        <v>12.67</v>
-      </c>
-      <c r="H12" s="47">
-        <v>88.69</v>
-      </c>
+      <c r="G12" s="41">
+        <f t="shared" si="0"/>
+        <v>134.67999999999998</v>
+      </c>
+      <c r="H12" s="50"/>
       <c r="I12" s="5"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -7398,11 +7390,10 @@
         <v>12.3874</v>
       </c>
       <c r="R12" s="36">
-        <v>35</v>
-      </c>
-      <c r="S12" s="36">
-        <v>315</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>111.4866</v>
+      </c>
+      <c r="S12" s="52"/>
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
@@ -7425,18 +7416,17 @@
       <c r="D13" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="41">
         <v>40</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="41">
         <v>62.42</v>
       </c>
-      <c r="G13" s="47">
-        <v>40</v>
-      </c>
-      <c r="H13" s="47">
-        <v>200</v>
-      </c>
+      <c r="G13" s="41">
+        <f t="shared" si="0"/>
+        <v>312.10000000000002</v>
+      </c>
+      <c r="H13" s="50"/>
       <c r="I13" s="5"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -7459,11 +7449,10 @@
         <v>15.045</v>
       </c>
       <c r="R13" s="36">
-        <v>40</v>
-      </c>
-      <c r="S13" s="36">
-        <v>240</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>90.27</v>
+      </c>
+      <c r="S13" s="52"/>
       <c r="U13" s="24"/>
       <c r="V13" s="24"/>
       <c r="W13" s="24"/>
@@ -7486,18 +7475,17 @@
       <c r="D14" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="41">
         <v>35.19</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="41">
         <v>44.95</v>
       </c>
-      <c r="G14" s="47">
-        <v>35.19</v>
-      </c>
-      <c r="H14" s="47">
-        <v>175.95</v>
-      </c>
+      <c r="G14" s="41">
+        <f t="shared" si="0"/>
+        <v>224.75</v>
+      </c>
+      <c r="H14" s="50"/>
       <c r="I14" s="5"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -7520,11 +7508,10 @@
         <v>4.1326999999999998</v>
       </c>
       <c r="R14" s="36">
-        <v>20</v>
-      </c>
-      <c r="S14" s="36">
-        <v>120</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>24.796199999999999</v>
+      </c>
+      <c r="S14" s="52"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
@@ -7547,18 +7534,17 @@
       <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="41">
         <v>15.72</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="41">
         <v>27.37</v>
       </c>
-      <c r="G15" s="47">
-        <v>15.72</v>
-      </c>
-      <c r="H15" s="47">
-        <v>62.88</v>
-      </c>
+      <c r="G15" s="41">
+        <f t="shared" si="0"/>
+        <v>109.48</v>
+      </c>
+      <c r="H15" s="50"/>
       <c r="I15" s="5"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -7581,11 +7567,10 @@
         <v>23.408999999999999</v>
       </c>
       <c r="R15" s="36">
-        <v>75</v>
-      </c>
-      <c r="S15" s="36">
-        <v>375</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>117.04499999999999</v>
+      </c>
+      <c r="S15" s="52"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
       <c r="W15" s="24"/>
@@ -7608,18 +7593,17 @@
       <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="41">
         <v>14.555400000000001</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="41">
         <v>25.419499999999999</v>
       </c>
-      <c r="G16" s="47">
-        <v>14.555400000000001</v>
-      </c>
-      <c r="H16" s="47">
-        <v>58.221600000000002</v>
-      </c>
+      <c r="G16" s="41">
+        <f t="shared" si="0"/>
+        <v>101.678</v>
+      </c>
+      <c r="H16" s="50"/>
       <c r="I16" s="5"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -7642,11 +7626,10 @@
         <v>12.3874</v>
       </c>
       <c r="R16" s="36">
-        <v>35</v>
-      </c>
-      <c r="S16" s="36">
-        <v>140</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>49.549599999999998</v>
+      </c>
+      <c r="S16" s="52"/>
       <c r="U16" s="24"/>
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
@@ -7669,18 +7652,17 @@
       <c r="D17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="41">
         <v>40</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="41">
         <v>53.94</v>
       </c>
-      <c r="G17" s="47">
-        <v>40</v>
-      </c>
-      <c r="H17" s="47">
-        <v>120</v>
-      </c>
+      <c r="G17" s="41">
+        <f t="shared" si="0"/>
+        <v>161.82</v>
+      </c>
+      <c r="H17" s="50"/>
       <c r="I17" s="5"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -7703,11 +7685,10 @@
         <v>12.561199999999999</v>
       </c>
       <c r="R17" s="36">
-        <v>30</v>
-      </c>
-      <c r="S17" s="36">
-        <v>120</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>50.244799999999998</v>
+      </c>
+      <c r="S17" s="52"/>
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
@@ -7730,18 +7711,17 @@
       <c r="D18" s="3">
         <v>3</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="41">
         <v>45.39</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="41">
         <v>52.74</v>
       </c>
-      <c r="G18" s="47">
-        <v>45.39</v>
-      </c>
-      <c r="H18" s="47">
-        <v>136.16999999999999</v>
-      </c>
+      <c r="G18" s="41">
+        <f t="shared" si="0"/>
+        <v>158.22</v>
+      </c>
+      <c r="H18" s="50"/>
       <c r="I18" s="5"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -7764,11 +7744,10 @@
         <v>33.480899999999998</v>
       </c>
       <c r="R18" s="36">
-        <v>80</v>
-      </c>
-      <c r="S18" s="36">
-        <v>320</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>133.92359999999999</v>
+      </c>
+      <c r="S18" s="52"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
@@ -7791,18 +7770,17 @@
       <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="41">
         <v>15.72</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="41">
         <v>21.37</v>
       </c>
-      <c r="G19" s="47">
-        <v>15.72</v>
-      </c>
-      <c r="H19" s="47">
-        <v>47.16</v>
-      </c>
+      <c r="G19" s="41">
+        <f t="shared" si="0"/>
+        <v>64.11</v>
+      </c>
+      <c r="H19" s="50"/>
       <c r="I19" s="5"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -7825,11 +7803,10 @@
         <v>15.709</v>
       </c>
       <c r="R19" s="36">
-        <v>45</v>
-      </c>
-      <c r="S19" s="36">
-        <v>135</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>47.126999999999995</v>
+      </c>
+      <c r="S19" s="52"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
@@ -7852,18 +7829,17 @@
       <c r="D20" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="47">
+      <c r="E20" s="41">
         <v>24</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="41">
         <v>33.689700000000002</v>
       </c>
-      <c r="G20" s="47">
-        <v>24</v>
-      </c>
-      <c r="H20" s="47">
-        <v>72</v>
-      </c>
+      <c r="G20" s="41">
+        <f t="shared" si="0"/>
+        <v>101.06910000000001</v>
+      </c>
+      <c r="H20" s="50"/>
       <c r="I20" s="5"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -7886,11 +7862,10 @@
         <v>12.561199999999999</v>
       </c>
       <c r="R20" s="36">
-        <v>30</v>
-      </c>
-      <c r="S20" s="36">
-        <v>60</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>25.122399999999999</v>
+      </c>
+      <c r="S20" s="52"/>
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
@@ -7913,18 +7888,17 @@
       <c r="D21" s="3">
         <v>22</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="41">
         <v>12.19</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="41">
         <v>20.64</v>
       </c>
-      <c r="G21" s="47">
-        <v>12.19</v>
-      </c>
-      <c r="H21" s="47">
-        <v>36.57</v>
-      </c>
+      <c r="G21" s="41">
+        <f t="shared" si="0"/>
+        <v>61.92</v>
+      </c>
+      <c r="H21" s="50"/>
       <c r="I21" s="5"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -7947,11 +7921,10 @@
         <v>15.2288</v>
       </c>
       <c r="R21" s="36">
-        <v>45</v>
-      </c>
-      <c r="S21" s="36">
-        <v>90</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>30.457599999999999</v>
+      </c>
+      <c r="S21" s="52"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
@@ -7974,18 +7947,17 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E22" s="41">
         <v>17.649999999999999</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="41">
         <v>40.29</v>
       </c>
-      <c r="G22" s="47">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="H22" s="47">
-        <v>35.299999999999997</v>
-      </c>
+      <c r="G22" s="41">
+        <f t="shared" si="0"/>
+        <v>80.58</v>
+      </c>
+      <c r="H22" s="50"/>
       <c r="I22" s="5"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -8008,11 +7980,10 @@
         <v>45.908999999999999</v>
       </c>
       <c r="R22" s="36">
-        <v>90</v>
-      </c>
-      <c r="S22" s="36">
-        <v>180</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>91.817999999999998</v>
+      </c>
+      <c r="S22" s="52"/>
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
       <c r="W22" s="24"/>
@@ -8035,18 +8006,17 @@
       <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="47">
+      <c r="E23" s="41">
         <v>45.39</v>
       </c>
-      <c r="F23" s="47">
+      <c r="F23" s="41">
         <v>54.47</v>
       </c>
-      <c r="G23" s="47">
-        <v>45.39</v>
-      </c>
-      <c r="H23" s="47">
-        <v>90.78</v>
-      </c>
+      <c r="G23" s="41">
+        <f t="shared" si="0"/>
+        <v>108.94</v>
+      </c>
+      <c r="H23" s="50"/>
       <c r="I23" s="5"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -8069,11 +8039,10 @@
         <v>29.135300000000001</v>
       </c>
       <c r="R23" s="36">
-        <v>64</v>
-      </c>
-      <c r="S23" s="36">
-        <v>128</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>58.270600000000002</v>
+      </c>
+      <c r="S23" s="52"/>
       <c r="U23" s="24"/>
       <c r="V23" s="24"/>
       <c r="W23" s="24"/>
@@ -8096,18 +8065,17 @@
       <c r="D24" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="41">
         <v>23</v>
       </c>
-      <c r="F24" s="47">
+      <c r="F24" s="41">
         <v>36.7211</v>
       </c>
-      <c r="G24" s="47">
-        <v>23</v>
-      </c>
-      <c r="H24" s="47">
-        <v>46</v>
-      </c>
+      <c r="G24" s="41">
+        <f t="shared" si="0"/>
+        <v>73.4422</v>
+      </c>
+      <c r="H24" s="50"/>
       <c r="I24" s="5"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -8130,11 +8098,10 @@
         <v>25.925000000000001</v>
       </c>
       <c r="R24" s="36">
-        <v>56</v>
-      </c>
-      <c r="S24" s="36">
-        <v>112</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>51.85</v>
+      </c>
+      <c r="S24" s="52"/>
       <c r="U24" s="24"/>
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
@@ -8157,18 +8124,17 @@
       <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="47">
+      <c r="E25" s="41">
         <v>15.72</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="41">
         <v>23.88</v>
       </c>
-      <c r="G25" s="47">
-        <v>15.72</v>
-      </c>
-      <c r="H25" s="47">
-        <v>31.44</v>
-      </c>
+      <c r="G25" s="41">
+        <f t="shared" si="0"/>
+        <v>47.76</v>
+      </c>
+      <c r="H25" s="50"/>
       <c r="I25" s="5"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -8191,11 +8157,10 @@
         <v>15.6813</v>
       </c>
       <c r="R25" s="36">
-        <v>40</v>
-      </c>
-      <c r="S25" s="36">
-        <v>80</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>31.3626</v>
+      </c>
+      <c r="S25" s="52"/>
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
@@ -8218,18 +8183,17 @@
       <c r="D26" s="3">
         <v>2</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="41">
         <v>14.31</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="41">
         <v>23.09</v>
       </c>
-      <c r="G26" s="47">
-        <v>14.31</v>
-      </c>
-      <c r="H26" s="47">
-        <v>28.62</v>
-      </c>
+      <c r="G26" s="41">
+        <f t="shared" si="0"/>
+        <v>46.18</v>
+      </c>
+      <c r="H26" s="50"/>
       <c r="I26" s="5"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -8252,11 +8216,10 @@
         <v>32.889000000000003</v>
       </c>
       <c r="R26" s="36">
-        <v>75</v>
-      </c>
-      <c r="S26" s="36">
-        <v>75</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>32.889000000000003</v>
+      </c>
+      <c r="S26" s="52"/>
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
@@ -8279,18 +8242,17 @@
       <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="41">
         <v>14.31</v>
       </c>
-      <c r="F27" s="47">
+      <c r="F27" s="41">
         <v>23.49</v>
       </c>
-      <c r="G27" s="47">
-        <v>14.31</v>
-      </c>
-      <c r="H27" s="47">
-        <v>28.62</v>
-      </c>
+      <c r="G27" s="41">
+        <f t="shared" si="0"/>
+        <v>46.98</v>
+      </c>
+      <c r="H27" s="50"/>
       <c r="I27" s="5"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -8313,11 +8275,10 @@
         <v>13.609</v>
       </c>
       <c r="R27" s="36">
-        <v>30</v>
-      </c>
-      <c r="S27" s="36">
-        <v>30</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>13.609</v>
+      </c>
+      <c r="S27" s="52"/>
       <c r="U27" s="24"/>
       <c r="V27" s="24"/>
       <c r="W27" s="24"/>
@@ -8340,18 +8301,17 @@
       <c r="D28" s="3">
         <v>19</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="41">
         <v>18.96</v>
       </c>
-      <c r="F28" s="47">
+      <c r="F28" s="41">
         <v>31.58</v>
       </c>
-      <c r="G28" s="47">
-        <v>18.96</v>
-      </c>
-      <c r="H28" s="47">
-        <v>37.92</v>
-      </c>
+      <c r="G28" s="41">
+        <f t="shared" si="0"/>
+        <v>63.16</v>
+      </c>
+      <c r="H28" s="50"/>
       <c r="I28" s="5"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -8374,11 +8334,10 @@
         <v>13.609</v>
       </c>
       <c r="R28" s="36">
-        <v>30</v>
-      </c>
-      <c r="S28" s="36">
-        <v>30</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>13.609</v>
+      </c>
+      <c r="S28" s="52"/>
       <c r="U28" s="24"/>
       <c r="V28" s="24"/>
       <c r="W28" s="24"/>
@@ -8401,18 +8360,17 @@
       <c r="D29" s="3">
         <v>22</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="41">
         <v>11.99</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="41">
         <v>20.43</v>
       </c>
-      <c r="G29" s="47">
-        <v>11.99</v>
-      </c>
-      <c r="H29" s="47">
-        <v>23.98</v>
-      </c>
+      <c r="G29" s="41">
+        <f t="shared" si="0"/>
+        <v>40.86</v>
+      </c>
+      <c r="H29" s="50"/>
       <c r="I29" s="5"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -8435,11 +8393,10 @@
         <v>42.3491</v>
       </c>
       <c r="R29" s="36">
-        <v>90</v>
-      </c>
-      <c r="S29" s="36">
-        <v>90</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>42.3491</v>
+      </c>
+      <c r="S29" s="52"/>
       <c r="U29" s="24"/>
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
@@ -8462,18 +8419,17 @@
       <c r="D30" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="41">
         <v>23</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="41">
         <v>32.69</v>
       </c>
-      <c r="G30" s="47">
-        <v>23</v>
-      </c>
-      <c r="H30" s="47">
-        <v>46</v>
-      </c>
+      <c r="G30" s="41">
+        <f t="shared" si="0"/>
+        <v>65.38</v>
+      </c>
+      <c r="H30" s="50"/>
       <c r="I30" s="5"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -8496,11 +8452,10 @@
         <v>15.709</v>
       </c>
       <c r="R30" s="36">
-        <v>40</v>
-      </c>
-      <c r="S30" s="36">
-        <v>40</v>
-      </c>
+        <f>M30*Q30</f>
+        <v>15.709</v>
+      </c>
+      <c r="S30" s="52"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -8515,18 +8470,17 @@
       <c r="D31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="47">
+      <c r="E31" s="41">
         <v>13.25</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F31" s="41">
         <v>26.34</v>
       </c>
-      <c r="G31" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H31" s="47">
-        <v>26.5</v>
-      </c>
+      <c r="G31" s="41">
+        <f t="shared" si="0"/>
+        <v>52.68</v>
+      </c>
+      <c r="H31" s="50"/>
       <c r="I31" s="5"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -8549,11 +8503,10 @@
         <v>25.859000000000002</v>
       </c>
       <c r="R31" s="36">
-        <v>65</v>
-      </c>
-      <c r="S31" s="36">
-        <v>65</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>25.859000000000002</v>
+      </c>
+      <c r="S31" s="52"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -8568,18 +8521,17 @@
       <c r="D32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="41">
         <v>13.25</v>
       </c>
-      <c r="F32" s="47">
+      <c r="F32" s="41">
         <v>23.35</v>
       </c>
-      <c r="G32" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H32" s="47">
-        <v>26.5</v>
-      </c>
+      <c r="G32" s="41">
+        <f t="shared" si="0"/>
+        <v>46.7</v>
+      </c>
+      <c r="H32" s="50"/>
       <c r="I32" s="5"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -8602,11 +8554,10 @@
         <v>11.613899999999999</v>
       </c>
       <c r="R32" s="36">
-        <v>40</v>
-      </c>
-      <c r="S32" s="36">
-        <v>40</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>11.613899999999999</v>
+      </c>
+      <c r="S32" s="52"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -8621,18 +8572,17 @@
       <c r="D33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="41">
         <v>15</v>
       </c>
-      <c r="F33" s="47">
+      <c r="F33" s="41">
         <v>28.15</v>
       </c>
-      <c r="G33" s="47">
-        <v>15</v>
-      </c>
-      <c r="H33" s="47">
-        <v>30</v>
-      </c>
+      <c r="G33" s="41">
+        <f t="shared" si="0"/>
+        <v>56.3</v>
+      </c>
+      <c r="H33" s="50"/>
       <c r="I33" s="5"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -8655,11 +8605,10 @@
         <v>11.613899999999999</v>
       </c>
       <c r="R33" s="36">
-        <v>35</v>
-      </c>
-      <c r="S33" s="36">
-        <v>35</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>11.613899999999999</v>
+      </c>
+      <c r="S33" s="52"/>
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
       <c r="Y33" s="24"/>
@@ -8678,18 +8627,17 @@
       <c r="D34" s="3">
         <v>22</v>
       </c>
-      <c r="E34" s="47">
+      <c r="E34" s="41">
         <v>11.193</v>
       </c>
-      <c r="F34" s="47">
+      <c r="F34" s="41">
         <v>19.637499999999999</v>
       </c>
-      <c r="G34" s="47">
-        <v>11.193</v>
-      </c>
-      <c r="H34" s="47">
-        <v>22.385999999999999</v>
-      </c>
+      <c r="G34" s="41">
+        <f t="shared" si="0"/>
+        <v>39.274999999999999</v>
+      </c>
+      <c r="H34" s="50"/>
       <c r="I34" s="5"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -8719,18 +8667,17 @@
       <c r="D35" s="3">
         <v>2</v>
       </c>
-      <c r="E35" s="47">
+      <c r="E35" s="41">
         <v>23.46</v>
       </c>
-      <c r="F35" s="47">
+      <c r="F35" s="41">
         <v>31.468399999999999</v>
       </c>
-      <c r="G35" s="47">
-        <v>23.46</v>
-      </c>
-      <c r="H35" s="47">
-        <v>23.46</v>
-      </c>
+      <c r="G35" s="41">
+        <f t="shared" si="0"/>
+        <v>31.468399999999999</v>
+      </c>
+      <c r="H35" s="50"/>
       <c r="I35" s="5"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -8760,18 +8707,17 @@
       <c r="D36" s="3">
         <v>2</v>
       </c>
-      <c r="E36" s="47">
+      <c r="E36" s="41">
         <v>12.3</v>
       </c>
-      <c r="F36" s="47">
+      <c r="F36" s="41">
         <v>24.4</v>
       </c>
-      <c r="G36" s="47">
-        <v>12.3</v>
-      </c>
-      <c r="H36" s="47">
-        <v>12.3</v>
-      </c>
+      <c r="G36" s="41">
+        <f t="shared" si="0"/>
+        <v>24.4</v>
+      </c>
+      <c r="H36" s="50"/>
       <c r="I36" s="5"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -8801,18 +8747,17 @@
       <c r="D37" s="3">
         <v>4</v>
       </c>
-      <c r="E37" s="47">
+      <c r="E37" s="41">
         <v>53.55</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F37" s="41">
         <v>60.65</v>
       </c>
-      <c r="G37" s="47">
-        <v>53.55</v>
-      </c>
-      <c r="H37" s="47">
-        <v>53.55</v>
-      </c>
+      <c r="G37" s="41">
+        <f t="shared" si="0"/>
+        <v>60.65</v>
+      </c>
+      <c r="H37" s="50"/>
       <c r="I37" s="5"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -8841,18 +8786,17 @@
       <c r="D38" s="3">
         <v>4</v>
       </c>
-      <c r="E38" s="47">
+      <c r="E38" s="41">
         <v>66.3</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="41">
         <v>73.319999999999993</v>
       </c>
-      <c r="G38" s="47">
-        <v>66.3</v>
-      </c>
-      <c r="H38" s="47">
-        <v>66.3</v>
-      </c>
+      <c r="G38" s="41">
+        <f t="shared" si="0"/>
+        <v>73.319999999999993</v>
+      </c>
+      <c r="H38" s="50"/>
       <c r="I38" s="5"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -8879,18 +8823,17 @@
       <c r="D39" s="3">
         <v>7</v>
       </c>
-      <c r="E39" s="47">
+      <c r="E39" s="41">
         <v>26.5</v>
       </c>
-      <c r="F39" s="47">
+      <c r="F39" s="41">
         <v>36.1496</v>
       </c>
-      <c r="G39" s="47">
-        <v>26.5</v>
-      </c>
-      <c r="H39" s="47">
-        <v>26.5</v>
-      </c>
+      <c r="G39" s="41">
+        <f t="shared" si="0"/>
+        <v>36.1496</v>
+      </c>
+      <c r="H39" s="50"/>
       <c r="I39"/>
       <c r="O39" s="3" t="s">
         <v>20</v>
@@ -8919,18 +8862,17 @@
       <c r="D40" s="3">
         <v>7</v>
       </c>
-      <c r="E40" s="47">
+      <c r="E40" s="41">
         <v>26.5</v>
       </c>
-      <c r="F40" s="47">
+      <c r="F40" s="41">
         <v>50.839300000000001</v>
       </c>
-      <c r="G40" s="47">
-        <v>26.5</v>
-      </c>
-      <c r="H40" s="47">
-        <v>26.5</v>
-      </c>
+      <c r="G40" s="41">
+        <f t="shared" si="0"/>
+        <v>50.839300000000001</v>
+      </c>
+      <c r="H40" s="50"/>
       <c r="I40"/>
       <c r="O40" s="3" t="s">
         <v>22</v>
@@ -8959,18 +8901,17 @@
       <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="47">
+      <c r="E41" s="41">
         <v>85.28</v>
       </c>
-      <c r="F41" s="47">
+      <c r="F41" s="41">
         <v>93.844999999999999</v>
       </c>
-      <c r="G41" s="47">
-        <v>85.28</v>
-      </c>
-      <c r="H41" s="47">
-        <v>85.28</v>
-      </c>
+      <c r="G41" s="41">
+        <f t="shared" si="0"/>
+        <v>93.844999999999999</v>
+      </c>
+      <c r="H41" s="50"/>
       <c r="I41"/>
       <c r="O41" s="3" t="s">
         <v>170</v>
@@ -8999,18 +8940,17 @@
       <c r="D42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="47">
+      <c r="E42" s="41">
         <v>13.25</v>
       </c>
-      <c r="F42" s="47">
+      <c r="F42" s="41">
         <v>24.41</v>
       </c>
-      <c r="G42" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H42" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G42" s="41">
+        <f t="shared" si="0"/>
+        <v>24.41</v>
+      </c>
+      <c r="H42" s="50"/>
       <c r="I42"/>
       <c r="O42" s="3" t="s">
         <v>21</v>
@@ -9039,18 +8979,17 @@
       <c r="D43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="47">
+      <c r="E43" s="41">
         <v>13.25</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="41">
         <v>22.82</v>
       </c>
-      <c r="G43" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H43" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G43" s="41">
+        <f t="shared" si="0"/>
+        <v>22.82</v>
+      </c>
+      <c r="H43" s="50"/>
       <c r="I43"/>
       <c r="O43" s="3" t="s">
         <v>54</v>
@@ -9079,18 +9018,17 @@
       <c r="D44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="47">
+      <c r="E44" s="41">
         <v>13.25</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F44" s="41">
         <v>22.2879</v>
       </c>
-      <c r="G44" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H44" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G44" s="41">
+        <f t="shared" si="0"/>
+        <v>22.2879</v>
+      </c>
+      <c r="H44" s="50"/>
       <c r="I44"/>
       <c r="O44" s="3" t="s">
         <v>25</v>
@@ -9119,18 +9057,17 @@
       <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="47">
+      <c r="E45" s="41">
         <v>13.25</v>
       </c>
-      <c r="F45" s="47">
+      <c r="F45" s="41">
         <v>21.477699999999999</v>
       </c>
-      <c r="G45" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H45" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G45" s="41">
+        <f>B45*F45</f>
+        <v>21.477699999999999</v>
+      </c>
+      <c r="H45" s="50"/>
       <c r="I45"/>
       <c r="O45" s="3" t="s">
         <v>121</v>
@@ -9159,18 +9096,17 @@
       <c r="D46" s="3">
         <v>19</v>
       </c>
-      <c r="E46" s="47">
+      <c r="E46" s="41">
         <v>18.008099999999999</v>
       </c>
-      <c r="F46" s="47">
+      <c r="F46" s="41">
         <v>27.285699999999999</v>
       </c>
-      <c r="G46" s="47">
-        <v>18.008099999999999</v>
-      </c>
-      <c r="H46" s="47">
-        <v>18.008099999999999</v>
-      </c>
+      <c r="G46" s="41">
+        <f t="shared" si="0"/>
+        <v>27.285699999999999</v>
+      </c>
+      <c r="H46" s="50"/>
       <c r="I46"/>
       <c r="O46" s="3" t="s">
         <v>52</v>
@@ -9195,18 +9131,17 @@
       <c r="D47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="47">
+      <c r="E47" s="41">
         <v>13.5</v>
       </c>
-      <c r="F47" s="47">
+      <c r="F47" s="41">
         <v>29.4359</v>
       </c>
-      <c r="G47" s="47">
-        <v>13.5</v>
-      </c>
-      <c r="H47" s="47">
-        <v>13.5</v>
-      </c>
+      <c r="G47" s="41">
+        <f t="shared" si="0"/>
+        <v>29.4359</v>
+      </c>
+      <c r="H47" s="50"/>
       <c r="I47"/>
       <c r="O47" s="3" t="s">
         <v>73</v>
@@ -9231,18 +9166,17 @@
       <c r="D48" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E48" s="47">
+      <c r="E48" s="41">
         <v>15</v>
       </c>
-      <c r="F48" s="47">
+      <c r="F48" s="41">
         <v>27.61</v>
       </c>
-      <c r="G48" s="47">
-        <v>15</v>
-      </c>
-      <c r="H48" s="47">
-        <v>15</v>
-      </c>
+      <c r="G48" s="41">
+        <f t="shared" si="0"/>
+        <v>27.61</v>
+      </c>
+      <c r="H48" s="50"/>
       <c r="I48"/>
       <c r="O48" s="3" t="s">
         <v>72</v>
@@ -9267,18 +9201,17 @@
       <c r="D49" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="47">
+      <c r="E49" s="41">
         <v>13.25</v>
       </c>
-      <c r="F49" s="47">
+      <c r="F49" s="41">
         <v>22.72</v>
       </c>
-      <c r="G49" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H49" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G49" s="41">
+        <f t="shared" si="0"/>
+        <v>22.72</v>
+      </c>
+      <c r="H49" s="50"/>
       <c r="I49"/>
       <c r="O49" s="3" t="s">
         <v>75</v>
@@ -9303,18 +9236,17 @@
       <c r="D50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="47">
+      <c r="E50" s="41">
         <v>13.25</v>
       </c>
-      <c r="F50" s="47">
+      <c r="F50" s="41">
         <v>23.35</v>
       </c>
-      <c r="G50" s="47">
-        <v>13.25</v>
-      </c>
-      <c r="H50" s="47">
-        <v>13.25</v>
-      </c>
+      <c r="G50" s="41">
+        <f t="shared" si="0"/>
+        <v>23.35</v>
+      </c>
+      <c r="H50" s="50"/>
       <c r="I50"/>
       <c r="O50" s="3" t="s">
         <v>171</v>
@@ -9379,8 +9311,8 @@
     <sortCondition descending="1" ref="B3:B50"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="L1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9433,38 +9365,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="P1" s="38" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="P1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="40"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="46"/>
     </row>
     <row r="2" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">

</xml_diff>